<commit_message>
calc average & compartments, add it to chernoff
</commit_message>
<xml_diff>
--- a/src/data/GUS/New/12 małopolskie.xlsx
+++ b/src/data/GUS/New/12 małopolskie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spis tablic List of tables" sheetId="17" r:id="rId1"/>
@@ -1947,6 +1947,7 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="25" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2055,7 +2056,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5310,42 +5310,42 @@
         <v>74</v>
       </c>
       <c r="C12" s="58"/>
-      <c r="D12" s="122" t="s">
+      <c r="D12" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="122"/>
-      <c r="K12" s="122"/>
-      <c r="L12" s="122"/>
-      <c r="M12" s="122"/>
-      <c r="N12" s="122"/>
-      <c r="O12" s="122"/>
-      <c r="P12" s="122"/>
-      <c r="Q12" s="122"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
+      <c r="L12" s="123"/>
+      <c r="M12" s="123"/>
+      <c r="N12" s="123"/>
+      <c r="O12" s="123"/>
+      <c r="P12" s="123"/>
+      <c r="Q12" s="123"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C13" s="58"/>
-      <c r="D13" s="123" t="s">
+      <c r="D13" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="123"/>
-      <c r="O13" s="123"/>
-      <c r="P13" s="123"/>
-      <c r="Q13" s="123"/>
-      <c r="R13" s="123"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="124"/>
+      <c r="O13" s="124"/>
+      <c r="P13" s="124"/>
+      <c r="Q13" s="124"/>
+      <c r="R13" s="124"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C14" s="58"/>
@@ -5355,46 +5355,46 @@
         <v>75</v>
       </c>
       <c r="C15" s="58"/>
-      <c r="D15" s="122" t="s">
+      <c r="D15" s="123" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="122"/>
-      <c r="I15" s="122"/>
-      <c r="J15" s="122"/>
-      <c r="K15" s="122"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="122"/>
-      <c r="O15" s="122"/>
-      <c r="P15" s="122"/>
-      <c r="Q15" s="122"/>
-      <c r="R15" s="122"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="123"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="123"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="123"/>
+      <c r="P15" s="123"/>
+      <c r="Q15" s="123"/>
+      <c r="R15" s="123"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="58"/>
-      <c r="D16" s="123" t="s">
+      <c r="D16" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="123"/>
-      <c r="K16" s="123"/>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
-      <c r="P16" s="123"/>
-      <c r="Q16" s="123"/>
-      <c r="R16" s="123"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="124"/>
+      <c r="Q16" s="124"/>
+      <c r="R16" s="124"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C17" s="58"/>
@@ -5404,43 +5404,43 @@
         <v>76</v>
       </c>
       <c r="C18" s="58"/>
-      <c r="D18" s="122" t="s">
+      <c r="D18" s="123" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="122"/>
-      <c r="H18" s="122"/>
-      <c r="I18" s="122"/>
-      <c r="J18" s="122"/>
-      <c r="K18" s="122"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
-      <c r="N18" s="122"/>
-      <c r="O18" s="122"/>
-      <c r="P18" s="122"/>
-      <c r="Q18" s="122"/>
-      <c r="R18" s="122"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="123"/>
+      <c r="I18" s="123"/>
+      <c r="J18" s="123"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
+      <c r="N18" s="123"/>
+      <c r="O18" s="123"/>
+      <c r="P18" s="123"/>
+      <c r="Q18" s="123"/>
+      <c r="R18" s="123"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C19" s="58"/>
-      <c r="D19" s="123" t="s">
+      <c r="D19" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="123"/>
-      <c r="J19" s="123"/>
-      <c r="K19" s="123"/>
-      <c r="L19" s="123"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="123"/>
-      <c r="O19" s="123"/>
-      <c r="P19" s="123"/>
-      <c r="Q19" s="123"/>
-      <c r="R19" s="123"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="124"/>
+      <c r="O19" s="124"/>
+      <c r="P19" s="124"/>
+      <c r="Q19" s="124"/>
+      <c r="R19" s="124"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C20" s="58"/>
@@ -5450,43 +5450,43 @@
         <v>77</v>
       </c>
       <c r="C21" s="58"/>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="122"/>
-      <c r="F21" s="122"/>
-      <c r="G21" s="122"/>
-      <c r="H21" s="122"/>
-      <c r="I21" s="122"/>
-      <c r="J21" s="122"/>
-      <c r="K21" s="122"/>
-      <c r="L21" s="122"/>
-      <c r="M21" s="122"/>
-      <c r="N21" s="122"/>
-      <c r="O21" s="122"/>
-      <c r="P21" s="122"/>
-      <c r="Q21" s="122"/>
-      <c r="R21" s="122"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
+      <c r="J21" s="123"/>
+      <c r="K21" s="123"/>
+      <c r="L21" s="123"/>
+      <c r="M21" s="123"/>
+      <c r="N21" s="123"/>
+      <c r="O21" s="123"/>
+      <c r="P21" s="123"/>
+      <c r="Q21" s="123"/>
+      <c r="R21" s="123"/>
     </row>
     <row r="22" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="58"/>
-      <c r="D22" s="123" t="s">
+      <c r="D22" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="123"/>
-      <c r="I22" s="123"/>
-      <c r="J22" s="123"/>
-      <c r="K22" s="123"/>
-      <c r="L22" s="123"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="123"/>
-      <c r="O22" s="123"/>
-      <c r="P22" s="123"/>
-      <c r="Q22" s="123"/>
-      <c r="R22" s="123"/>
+      <c r="E22" s="124"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="124"/>
+      <c r="H22" s="124"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
+      <c r="K22" s="124"/>
+      <c r="L22" s="124"/>
+      <c r="M22" s="124"/>
+      <c r="N22" s="124"/>
+      <c r="O22" s="124"/>
+      <c r="P22" s="124"/>
+      <c r="Q22" s="124"/>
+      <c r="R22" s="124"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="88"/>
@@ -5499,46 +5499,46 @@
         <v>90</v>
       </c>
       <c r="C24" s="58"/>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="123" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="122"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="122"/>
-      <c r="H24" s="122"/>
-      <c r="I24" s="122"/>
-      <c r="J24" s="122"/>
-      <c r="K24" s="122"/>
-      <c r="L24" s="122"/>
-      <c r="M24" s="122"/>
-      <c r="N24" s="122"/>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="123"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="123"/>
+      <c r="I24" s="123"/>
+      <c r="J24" s="123"/>
+      <c r="K24" s="123"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="123"/>
+      <c r="N24" s="123"/>
+      <c r="O24" s="123"/>
+      <c r="P24" s="123"/>
+      <c r="Q24" s="123"/>
+      <c r="R24" s="123"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="61" t="s">
         <v>96</v>
       </c>
       <c r="C25" s="58"/>
-      <c r="D25" s="123" t="s">
+      <c r="D25" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="123"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="123"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="123"/>
-      <c r="L25" s="123"/>
-      <c r="M25" s="123"/>
-      <c r="N25" s="123"/>
-      <c r="O25" s="123"/>
-      <c r="P25" s="123"/>
-      <c r="Q25" s="123"/>
-      <c r="R25" s="123"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="124"/>
+      <c r="I25" s="124"/>
+      <c r="J25" s="124"/>
+      <c r="K25" s="124"/>
+      <c r="L25" s="124"/>
+      <c r="M25" s="124"/>
+      <c r="N25" s="124"/>
+      <c r="O25" s="124"/>
+      <c r="P25" s="124"/>
+      <c r="Q25" s="124"/>
+      <c r="R25" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5582,14 +5582,14 @@
   <sheetPr codeName="Arkusz2">
     <tabColor rgb="FF66C2C9"/>
   </sheetPr>
-  <dimension ref="A1:AO313"/>
+  <dimension ref="A1:AO333"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C305" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5:A6"/>
       <selection pane="topRight" activeCell="A5" sqref="A5:A6"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:A6"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+      <selection pane="bottomRight" activeCell="H334" sqref="H334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5600,8 +5600,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="76" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="124"/>
-      <c r="B1" s="124"/>
+      <c r="A1" s="125"/>
+      <c r="B1" s="125"/>
       <c r="C1" s="73" t="s">
         <v>44</v>
       </c>
@@ -5645,10 +5645,10 @@
       <c r="AO1" s="77"/>
     </row>
     <row r="2" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="127"/>
+      <c r="B2" s="128"/>
       <c r="D2" s="26" t="s">
         <v>40</v>
       </c>
@@ -5691,10 +5691,10 @@
       <c r="AO2" s="24"/>
     </row>
     <row r="3" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="128"/>
+      <c r="B3" s="129"/>
       <c r="D3" s="22" t="s">
         <v>43</v>
       </c>
@@ -5995,7 +5995,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" s="125" t="s">
+      <c r="A8" s="126" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="71" t="s">
@@ -6120,7 +6120,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A9" s="125"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="9">
         <v>0</v>
       </c>
@@ -6243,7 +6243,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" s="125"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="9">
         <v>1</v>
       </c>
@@ -6366,7 +6366,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A11" s="125"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="9">
         <v>2</v>
       </c>
@@ -6489,7 +6489,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" s="125"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="9">
         <v>3</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="125"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="9">
         <v>4</v>
       </c>
@@ -6735,7 +6735,7 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" s="125"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="9">
         <v>5</v>
       </c>
@@ -6858,7 +6858,7 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A15" s="125"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="9">
         <v>6</v>
       </c>
@@ -6981,7 +6981,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" s="125"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="9">
         <v>7</v>
       </c>
@@ -7104,7 +7104,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A17" s="125"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="9">
         <v>8</v>
       </c>
@@ -7227,7 +7227,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A18" s="125"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="9">
         <v>9</v>
       </c>
@@ -7350,7 +7350,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A19" s="125"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="9">
         <v>10</v>
       </c>
@@ -7473,7 +7473,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A20" s="125"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="9">
         <v>11</v>
       </c>
@@ -7596,7 +7596,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A21" s="125"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="9">
         <v>12</v>
       </c>
@@ -7719,7 +7719,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A22" s="125"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="9">
         <v>13</v>
       </c>
@@ -7842,7 +7842,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A23" s="125"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="9">
         <v>14</v>
       </c>
@@ -7965,7 +7965,7 @@
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A24" s="125"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="9">
         <v>15</v>
       </c>
@@ -8088,7 +8088,7 @@
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A25" s="125"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="9">
         <v>16</v>
       </c>
@@ -8211,7 +8211,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A26" s="125"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="9">
         <v>17</v>
       </c>
@@ -8334,7 +8334,7 @@
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A27" s="125"/>
+      <c r="A27" s="126"/>
       <c r="B27" s="9">
         <v>18</v>
       </c>
@@ -8457,7 +8457,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A28" s="125"/>
+      <c r="A28" s="126"/>
       <c r="B28" s="9">
         <v>19</v>
       </c>
@@ -8580,7 +8580,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A29" s="125"/>
+      <c r="A29" s="126"/>
       <c r="B29" s="9">
         <v>20</v>
       </c>
@@ -8703,7 +8703,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A30" s="125"/>
+      <c r="A30" s="126"/>
       <c r="B30" s="9">
         <v>21</v>
       </c>
@@ -8826,7 +8826,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A31" s="125"/>
+      <c r="A31" s="126"/>
       <c r="B31" s="9">
         <v>22</v>
       </c>
@@ -8949,7 +8949,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A32" s="125"/>
+      <c r="A32" s="126"/>
       <c r="B32" s="9">
         <v>23</v>
       </c>
@@ -9072,7 +9072,7 @@
       </c>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A33" s="125"/>
+      <c r="A33" s="126"/>
       <c r="B33" s="9">
         <v>24</v>
       </c>
@@ -9195,7 +9195,7 @@
       </c>
     </row>
     <row r="34" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A34" s="125"/>
+      <c r="A34" s="126"/>
       <c r="B34" s="9">
         <v>25</v>
       </c>
@@ -9318,7 +9318,7 @@
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A35" s="125"/>
+      <c r="A35" s="126"/>
       <c r="B35" s="9">
         <v>26</v>
       </c>
@@ -9441,7 +9441,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A36" s="125"/>
+      <c r="A36" s="126"/>
       <c r="B36" s="9">
         <v>27</v>
       </c>
@@ -9564,7 +9564,7 @@
       </c>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A37" s="125"/>
+      <c r="A37" s="126"/>
       <c r="B37" s="9">
         <v>28</v>
       </c>
@@ -9687,7 +9687,7 @@
       </c>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A38" s="125"/>
+      <c r="A38" s="126"/>
       <c r="B38" s="9">
         <v>29</v>
       </c>
@@ -9810,7 +9810,7 @@
       </c>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A39" s="125"/>
+      <c r="A39" s="126"/>
       <c r="B39" s="9">
         <v>30</v>
       </c>
@@ -9933,7 +9933,7 @@
       </c>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A40" s="125"/>
+      <c r="A40" s="126"/>
       <c r="B40" s="9">
         <v>31</v>
       </c>
@@ -10056,7 +10056,7 @@
       </c>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A41" s="125"/>
+      <c r="A41" s="126"/>
       <c r="B41" s="9">
         <v>32</v>
       </c>
@@ -10179,7 +10179,7 @@
       </c>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A42" s="125"/>
+      <c r="A42" s="126"/>
       <c r="B42" s="9">
         <v>33</v>
       </c>
@@ -10302,7 +10302,7 @@
       </c>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A43" s="125"/>
+      <c r="A43" s="126"/>
       <c r="B43" s="9">
         <v>34</v>
       </c>
@@ -10425,7 +10425,7 @@
       </c>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A44" s="125"/>
+      <c r="A44" s="126"/>
       <c r="B44" s="9">
         <v>35</v>
       </c>
@@ -10548,7 +10548,7 @@
       </c>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A45" s="125"/>
+      <c r="A45" s="126"/>
       <c r="B45" s="9">
         <v>36</v>
       </c>
@@ -10671,7 +10671,7 @@
       </c>
     </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A46" s="125"/>
+      <c r="A46" s="126"/>
       <c r="B46" s="9">
         <v>37</v>
       </c>
@@ -10794,7 +10794,7 @@
       </c>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A47" s="125"/>
+      <c r="A47" s="126"/>
       <c r="B47" s="9">
         <v>38</v>
       </c>
@@ -10917,7 +10917,7 @@
       </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A48" s="125"/>
+      <c r="A48" s="126"/>
       <c r="B48" s="9">
         <v>39</v>
       </c>
@@ -11040,7 +11040,7 @@
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A49" s="125"/>
+      <c r="A49" s="126"/>
       <c r="B49" s="9">
         <v>40</v>
       </c>
@@ -11163,7 +11163,7 @@
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A50" s="125"/>
+      <c r="A50" s="126"/>
       <c r="B50" s="9">
         <v>41</v>
       </c>
@@ -11286,7 +11286,7 @@
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A51" s="125"/>
+      <c r="A51" s="126"/>
       <c r="B51" s="9">
         <v>42</v>
       </c>
@@ -11409,7 +11409,7 @@
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A52" s="125"/>
+      <c r="A52" s="126"/>
       <c r="B52" s="9">
         <v>43</v>
       </c>
@@ -11532,7 +11532,7 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A53" s="125"/>
+      <c r="A53" s="126"/>
       <c r="B53" s="9">
         <v>44</v>
       </c>
@@ -11655,7 +11655,7 @@
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A54" s="125"/>
+      <c r="A54" s="126"/>
       <c r="B54" s="9">
         <v>45</v>
       </c>
@@ -11778,7 +11778,7 @@
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A55" s="125"/>
+      <c r="A55" s="126"/>
       <c r="B55" s="9">
         <v>46</v>
       </c>
@@ -11901,7 +11901,7 @@
       </c>
     </row>
     <row r="56" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A56" s="125"/>
+      <c r="A56" s="126"/>
       <c r="B56" s="9">
         <v>47</v>
       </c>
@@ -12024,7 +12024,7 @@
       </c>
     </row>
     <row r="57" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A57" s="125"/>
+      <c r="A57" s="126"/>
       <c r="B57" s="9">
         <v>48</v>
       </c>
@@ -12147,7 +12147,7 @@
       </c>
     </row>
     <row r="58" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A58" s="125"/>
+      <c r="A58" s="126"/>
       <c r="B58" s="9">
         <v>49</v>
       </c>
@@ -12270,7 +12270,7 @@
       </c>
     </row>
     <row r="59" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A59" s="125"/>
+      <c r="A59" s="126"/>
       <c r="B59" s="9">
         <v>50</v>
       </c>
@@ -12393,7 +12393,7 @@
       </c>
     </row>
     <row r="60" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A60" s="125"/>
+      <c r="A60" s="126"/>
       <c r="B60" s="9">
         <v>51</v>
       </c>
@@ -12516,7 +12516,7 @@
       </c>
     </row>
     <row r="61" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A61" s="125"/>
+      <c r="A61" s="126"/>
       <c r="B61" s="9">
         <v>52</v>
       </c>
@@ -12639,7 +12639,7 @@
       </c>
     </row>
     <row r="62" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A62" s="125"/>
+      <c r="A62" s="126"/>
       <c r="B62" s="9">
         <v>53</v>
       </c>
@@ -12762,7 +12762,7 @@
       </c>
     </row>
     <row r="63" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A63" s="125"/>
+      <c r="A63" s="126"/>
       <c r="B63" s="9">
         <v>54</v>
       </c>
@@ -12885,7 +12885,7 @@
       </c>
     </row>
     <row r="64" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A64" s="125"/>
+      <c r="A64" s="126"/>
       <c r="B64" s="9">
         <v>55</v>
       </c>
@@ -13008,7 +13008,7 @@
       </c>
     </row>
     <row r="65" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A65" s="125"/>
+      <c r="A65" s="126"/>
       <c r="B65" s="9">
         <v>56</v>
       </c>
@@ -13131,7 +13131,7 @@
       </c>
     </row>
     <row r="66" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A66" s="125"/>
+      <c r="A66" s="126"/>
       <c r="B66" s="9">
         <v>57</v>
       </c>
@@ -13254,7 +13254,7 @@
       </c>
     </row>
     <row r="67" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A67" s="125"/>
+      <c r="A67" s="126"/>
       <c r="B67" s="9">
         <v>58</v>
       </c>
@@ -13377,7 +13377,7 @@
       </c>
     </row>
     <row r="68" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A68" s="125"/>
+      <c r="A68" s="126"/>
       <c r="B68" s="9">
         <v>59</v>
       </c>
@@ -13500,7 +13500,7 @@
       </c>
     </row>
     <row r="69" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A69" s="125"/>
+      <c r="A69" s="126"/>
       <c r="B69" s="9">
         <v>60</v>
       </c>
@@ -13623,7 +13623,7 @@
       </c>
     </row>
     <row r="70" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A70" s="125"/>
+      <c r="A70" s="126"/>
       <c r="B70" s="9">
         <v>61</v>
       </c>
@@ -13746,7 +13746,7 @@
       </c>
     </row>
     <row r="71" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A71" s="125"/>
+      <c r="A71" s="126"/>
       <c r="B71" s="9">
         <v>62</v>
       </c>
@@ -13869,7 +13869,7 @@
       </c>
     </row>
     <row r="72" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A72" s="125"/>
+      <c r="A72" s="126"/>
       <c r="B72" s="9">
         <v>63</v>
       </c>
@@ -13992,7 +13992,7 @@
       </c>
     </row>
     <row r="73" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A73" s="125"/>
+      <c r="A73" s="126"/>
       <c r="B73" s="9">
         <v>64</v>
       </c>
@@ -14115,7 +14115,7 @@
       </c>
     </row>
     <row r="74" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A74" s="125"/>
+      <c r="A74" s="126"/>
       <c r="B74" s="9">
         <v>65</v>
       </c>
@@ -14238,7 +14238,7 @@
       </c>
     </row>
     <row r="75" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A75" s="125"/>
+      <c r="A75" s="126"/>
       <c r="B75" s="9">
         <v>66</v>
       </c>
@@ -14361,7 +14361,7 @@
       </c>
     </row>
     <row r="76" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A76" s="125"/>
+      <c r="A76" s="126"/>
       <c r="B76" s="9">
         <v>67</v>
       </c>
@@ -14484,7 +14484,7 @@
       </c>
     </row>
     <row r="77" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A77" s="125"/>
+      <c r="A77" s="126"/>
       <c r="B77" s="9">
         <v>68</v>
       </c>
@@ -14607,7 +14607,7 @@
       </c>
     </row>
     <row r="78" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A78" s="125"/>
+      <c r="A78" s="126"/>
       <c r="B78" s="9">
         <v>69</v>
       </c>
@@ -14730,7 +14730,7 @@
       </c>
     </row>
     <row r="79" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A79" s="125"/>
+      <c r="A79" s="126"/>
       <c r="B79" s="9">
         <v>70</v>
       </c>
@@ -14853,7 +14853,7 @@
       </c>
     </row>
     <row r="80" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A80" s="125"/>
+      <c r="A80" s="126"/>
       <c r="B80" s="9">
         <v>71</v>
       </c>
@@ -14976,7 +14976,7 @@
       </c>
     </row>
     <row r="81" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A81" s="125"/>
+      <c r="A81" s="126"/>
       <c r="B81" s="9">
         <v>72</v>
       </c>
@@ -15099,7 +15099,7 @@
       </c>
     </row>
     <row r="82" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A82" s="125"/>
+      <c r="A82" s="126"/>
       <c r="B82" s="9">
         <v>73</v>
       </c>
@@ -15222,7 +15222,7 @@
       </c>
     </row>
     <row r="83" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A83" s="125"/>
+      <c r="A83" s="126"/>
       <c r="B83" s="9">
         <v>74</v>
       </c>
@@ -15345,7 +15345,7 @@
       </c>
     </row>
     <row r="84" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A84" s="125"/>
+      <c r="A84" s="126"/>
       <c r="B84" s="9">
         <v>75</v>
       </c>
@@ -15468,7 +15468,7 @@
       </c>
     </row>
     <row r="85" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A85" s="125"/>
+      <c r="A85" s="126"/>
       <c r="B85" s="9">
         <v>76</v>
       </c>
@@ -15591,7 +15591,7 @@
       </c>
     </row>
     <row r="86" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A86" s="125"/>
+      <c r="A86" s="126"/>
       <c r="B86" s="9">
         <v>77</v>
       </c>
@@ -15714,7 +15714,7 @@
       </c>
     </row>
     <row r="87" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A87" s="125"/>
+      <c r="A87" s="126"/>
       <c r="B87" s="9">
         <v>78</v>
       </c>
@@ -15837,7 +15837,7 @@
       </c>
     </row>
     <row r="88" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A88" s="125"/>
+      <c r="A88" s="126"/>
       <c r="B88" s="9">
         <v>79</v>
       </c>
@@ -15960,7 +15960,7 @@
       </c>
     </row>
     <row r="89" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A89" s="125"/>
+      <c r="A89" s="126"/>
       <c r="B89" s="9">
         <v>80</v>
       </c>
@@ -16083,7 +16083,7 @@
       </c>
     </row>
     <row r="90" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A90" s="125"/>
+      <c r="A90" s="126"/>
       <c r="B90" s="9">
         <v>81</v>
       </c>
@@ -16206,7 +16206,7 @@
       </c>
     </row>
     <row r="91" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A91" s="125"/>
+      <c r="A91" s="126"/>
       <c r="B91" s="9">
         <v>82</v>
       </c>
@@ -16329,7 +16329,7 @@
       </c>
     </row>
     <row r="92" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A92" s="125"/>
+      <c r="A92" s="126"/>
       <c r="B92" s="9">
         <v>83</v>
       </c>
@@ -16452,7 +16452,7 @@
       </c>
     </row>
     <row r="93" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A93" s="125"/>
+      <c r="A93" s="126"/>
       <c r="B93" s="9">
         <v>84</v>
       </c>
@@ -16575,7 +16575,7 @@
       </c>
     </row>
     <row r="94" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A94" s="125"/>
+      <c r="A94" s="126"/>
       <c r="B94" s="9">
         <v>85</v>
       </c>
@@ -16698,7 +16698,7 @@
       </c>
     </row>
     <row r="95" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A95" s="125"/>
+      <c r="A95" s="126"/>
       <c r="B95" s="9">
         <v>86</v>
       </c>
@@ -16821,7 +16821,7 @@
       </c>
     </row>
     <row r="96" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A96" s="125"/>
+      <c r="A96" s="126"/>
       <c r="B96" s="9">
         <v>87</v>
       </c>
@@ -16944,7 +16944,7 @@
       </c>
     </row>
     <row r="97" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A97" s="125"/>
+      <c r="A97" s="126"/>
       <c r="B97" s="9">
         <v>88</v>
       </c>
@@ -17067,7 +17067,7 @@
       </c>
     </row>
     <row r="98" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A98" s="125"/>
+      <c r="A98" s="126"/>
       <c r="B98" s="9">
         <v>89</v>
       </c>
@@ -17190,7 +17190,7 @@
       </c>
     </row>
     <row r="99" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A99" s="125"/>
+      <c r="A99" s="126"/>
       <c r="B99" s="9">
         <v>90</v>
       </c>
@@ -17313,7 +17313,7 @@
       </c>
     </row>
     <row r="100" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A100" s="125"/>
+      <c r="A100" s="126"/>
       <c r="B100" s="9">
         <v>91</v>
       </c>
@@ -17436,7 +17436,7 @@
       </c>
     </row>
     <row r="101" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A101" s="125"/>
+      <c r="A101" s="126"/>
       <c r="B101" s="9">
         <v>92</v>
       </c>
@@ -17559,7 +17559,7 @@
       </c>
     </row>
     <row r="102" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A102" s="125"/>
+      <c r="A102" s="126"/>
       <c r="B102" s="9">
         <v>93</v>
       </c>
@@ -17682,7 +17682,7 @@
       </c>
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A103" s="125"/>
+      <c r="A103" s="126"/>
       <c r="B103" s="9">
         <v>94</v>
       </c>
@@ -17805,7 +17805,7 @@
       </c>
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A104" s="125"/>
+      <c r="A104" s="126"/>
       <c r="B104" s="9">
         <v>95</v>
       </c>
@@ -17928,7 +17928,7 @@
       </c>
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A105" s="125"/>
+      <c r="A105" s="126"/>
       <c r="B105" s="9">
         <v>96</v>
       </c>
@@ -18051,7 +18051,7 @@
       </c>
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A106" s="125"/>
+      <c r="A106" s="126"/>
       <c r="B106" s="9">
         <v>97</v>
       </c>
@@ -18174,7 +18174,7 @@
       </c>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A107" s="125"/>
+      <c r="A107" s="126"/>
       <c r="B107" s="9">
         <v>98</v>
       </c>
@@ -18297,7 +18297,7 @@
       </c>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A108" s="125"/>
+      <c r="A108" s="126"/>
       <c r="B108" s="9">
         <v>99</v>
       </c>
@@ -18420,7 +18420,7 @@
       </c>
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A109" s="125"/>
+      <c r="A109" s="126"/>
       <c r="B109" s="9" t="s">
         <v>79</v>
       </c>
@@ -18543,7 +18543,7 @@
       </c>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A110" s="126" t="s">
+      <c r="A110" s="127" t="s">
         <v>50</v>
       </c>
       <c r="B110" s="71" t="s">
@@ -18668,7 +18668,7 @@
       </c>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A111" s="125"/>
+      <c r="A111" s="126"/>
       <c r="B111" s="9">
         <v>0</v>
       </c>
@@ -18791,7 +18791,7 @@
       </c>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A112" s="125"/>
+      <c r="A112" s="126"/>
       <c r="B112" s="9">
         <v>1</v>
       </c>
@@ -18914,7 +18914,7 @@
       </c>
     </row>
     <row r="113" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A113" s="125"/>
+      <c r="A113" s="126"/>
       <c r="B113" s="9">
         <v>2</v>
       </c>
@@ -19037,7 +19037,7 @@
       </c>
     </row>
     <row r="114" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A114" s="125"/>
+      <c r="A114" s="126"/>
       <c r="B114" s="9">
         <v>3</v>
       </c>
@@ -19160,7 +19160,7 @@
       </c>
     </row>
     <row r="115" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A115" s="125"/>
+      <c r="A115" s="126"/>
       <c r="B115" s="9">
         <v>4</v>
       </c>
@@ -19283,7 +19283,7 @@
       </c>
     </row>
     <row r="116" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A116" s="125"/>
+      <c r="A116" s="126"/>
       <c r="B116" s="9">
         <v>5</v>
       </c>
@@ -19406,7 +19406,7 @@
       </c>
     </row>
     <row r="117" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A117" s="125"/>
+      <c r="A117" s="126"/>
       <c r="B117" s="9">
         <v>6</v>
       </c>
@@ -19529,7 +19529,7 @@
       </c>
     </row>
     <row r="118" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A118" s="125"/>
+      <c r="A118" s="126"/>
       <c r="B118" s="9">
         <v>7</v>
       </c>
@@ -19652,7 +19652,7 @@
       </c>
     </row>
     <row r="119" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A119" s="125"/>
+      <c r="A119" s="126"/>
       <c r="B119" s="9">
         <v>8</v>
       </c>
@@ -19775,7 +19775,7 @@
       </c>
     </row>
     <row r="120" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A120" s="125"/>
+      <c r="A120" s="126"/>
       <c r="B120" s="9">
         <v>9</v>
       </c>
@@ -19898,7 +19898,7 @@
       </c>
     </row>
     <row r="121" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A121" s="125"/>
+      <c r="A121" s="126"/>
       <c r="B121" s="9">
         <v>10</v>
       </c>
@@ -20021,7 +20021,7 @@
       </c>
     </row>
     <row r="122" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A122" s="125"/>
+      <c r="A122" s="126"/>
       <c r="B122" s="9">
         <v>11</v>
       </c>
@@ -20144,7 +20144,7 @@
       </c>
     </row>
     <row r="123" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A123" s="125"/>
+      <c r="A123" s="126"/>
       <c r="B123" s="9">
         <v>12</v>
       </c>
@@ -20267,7 +20267,7 @@
       </c>
     </row>
     <row r="124" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A124" s="125"/>
+      <c r="A124" s="126"/>
       <c r="B124" s="9">
         <v>13</v>
       </c>
@@ -20390,7 +20390,7 @@
       </c>
     </row>
     <row r="125" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A125" s="125"/>
+      <c r="A125" s="126"/>
       <c r="B125" s="9">
         <v>14</v>
       </c>
@@ -20513,7 +20513,7 @@
       </c>
     </row>
     <row r="126" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A126" s="125"/>
+      <c r="A126" s="126"/>
       <c r="B126" s="9">
         <v>15</v>
       </c>
@@ -20636,7 +20636,7 @@
       </c>
     </row>
     <row r="127" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A127" s="125"/>
+      <c r="A127" s="126"/>
       <c r="B127" s="9">
         <v>16</v>
       </c>
@@ -20759,7 +20759,7 @@
       </c>
     </row>
     <row r="128" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A128" s="125"/>
+      <c r="A128" s="126"/>
       <c r="B128" s="9">
         <v>17</v>
       </c>
@@ -20882,7 +20882,7 @@
       </c>
     </row>
     <row r="129" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A129" s="125"/>
+      <c r="A129" s="126"/>
       <c r="B129" s="9">
         <v>18</v>
       </c>
@@ -21005,7 +21005,7 @@
       </c>
     </row>
     <row r="130" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A130" s="125"/>
+      <c r="A130" s="126"/>
       <c r="B130" s="9">
         <v>19</v>
       </c>
@@ -21128,7 +21128,7 @@
       </c>
     </row>
     <row r="131" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A131" s="125"/>
+      <c r="A131" s="126"/>
       <c r="B131" s="9">
         <v>20</v>
       </c>
@@ -21251,7 +21251,7 @@
       </c>
     </row>
     <row r="132" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A132" s="125"/>
+      <c r="A132" s="126"/>
       <c r="B132" s="9">
         <v>21</v>
       </c>
@@ -21374,7 +21374,7 @@
       </c>
     </row>
     <row r="133" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A133" s="125"/>
+      <c r="A133" s="126"/>
       <c r="B133" s="9">
         <v>22</v>
       </c>
@@ -21497,7 +21497,7 @@
       </c>
     </row>
     <row r="134" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A134" s="125"/>
+      <c r="A134" s="126"/>
       <c r="B134" s="9">
         <v>23</v>
       </c>
@@ -21620,7 +21620,7 @@
       </c>
     </row>
     <row r="135" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A135" s="125"/>
+      <c r="A135" s="126"/>
       <c r="B135" s="9">
         <v>24</v>
       </c>
@@ -21743,7 +21743,7 @@
       </c>
     </row>
     <row r="136" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A136" s="125"/>
+      <c r="A136" s="126"/>
       <c r="B136" s="9">
         <v>25</v>
       </c>
@@ -21866,7 +21866,7 @@
       </c>
     </row>
     <row r="137" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A137" s="125"/>
+      <c r="A137" s="126"/>
       <c r="B137" s="9">
         <v>26</v>
       </c>
@@ -21989,7 +21989,7 @@
       </c>
     </row>
     <row r="138" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A138" s="125"/>
+      <c r="A138" s="126"/>
       <c r="B138" s="9">
         <v>27</v>
       </c>
@@ -22112,7 +22112,7 @@
       </c>
     </row>
     <row r="139" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A139" s="125"/>
+      <c r="A139" s="126"/>
       <c r="B139" s="9">
         <v>28</v>
       </c>
@@ -22235,7 +22235,7 @@
       </c>
     </row>
     <row r="140" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A140" s="125"/>
+      <c r="A140" s="126"/>
       <c r="B140" s="9">
         <v>29</v>
       </c>
@@ -22358,7 +22358,7 @@
       </c>
     </row>
     <row r="141" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A141" s="125"/>
+      <c r="A141" s="126"/>
       <c r="B141" s="9">
         <v>30</v>
       </c>
@@ -22481,7 +22481,7 @@
       </c>
     </row>
     <row r="142" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A142" s="125"/>
+      <c r="A142" s="126"/>
       <c r="B142" s="9">
         <v>31</v>
       </c>
@@ -22604,7 +22604,7 @@
       </c>
     </row>
     <row r="143" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A143" s="125"/>
+      <c r="A143" s="126"/>
       <c r="B143" s="9">
         <v>32</v>
       </c>
@@ -22727,7 +22727,7 @@
       </c>
     </row>
     <row r="144" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A144" s="125"/>
+      <c r="A144" s="126"/>
       <c r="B144" s="9">
         <v>33</v>
       </c>
@@ -22850,7 +22850,7 @@
       </c>
     </row>
     <row r="145" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A145" s="125"/>
+      <c r="A145" s="126"/>
       <c r="B145" s="9">
         <v>34</v>
       </c>
@@ -22973,7 +22973,7 @@
       </c>
     </row>
     <row r="146" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A146" s="125"/>
+      <c r="A146" s="126"/>
       <c r="B146" s="9">
         <v>35</v>
       </c>
@@ -23096,7 +23096,7 @@
       </c>
     </row>
     <row r="147" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A147" s="125"/>
+      <c r="A147" s="126"/>
       <c r="B147" s="9">
         <v>36</v>
       </c>
@@ -23219,7 +23219,7 @@
       </c>
     </row>
     <row r="148" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A148" s="125"/>
+      <c r="A148" s="126"/>
       <c r="B148" s="9">
         <v>37</v>
       </c>
@@ -23342,7 +23342,7 @@
       </c>
     </row>
     <row r="149" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A149" s="125"/>
+      <c r="A149" s="126"/>
       <c r="B149" s="9">
         <v>38</v>
       </c>
@@ -23465,7 +23465,7 @@
       </c>
     </row>
     <row r="150" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A150" s="125"/>
+      <c r="A150" s="126"/>
       <c r="B150" s="9">
         <v>39</v>
       </c>
@@ -23588,7 +23588,7 @@
       </c>
     </row>
     <row r="151" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A151" s="125"/>
+      <c r="A151" s="126"/>
       <c r="B151" s="9">
         <v>40</v>
       </c>
@@ -23711,7 +23711,7 @@
       </c>
     </row>
     <row r="152" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A152" s="125"/>
+      <c r="A152" s="126"/>
       <c r="B152" s="9">
         <v>41</v>
       </c>
@@ -23834,7 +23834,7 @@
       </c>
     </row>
     <row r="153" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A153" s="125"/>
+      <c r="A153" s="126"/>
       <c r="B153" s="9">
         <v>42</v>
       </c>
@@ -23957,7 +23957,7 @@
       </c>
     </row>
     <row r="154" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A154" s="125"/>
+      <c r="A154" s="126"/>
       <c r="B154" s="9">
         <v>43</v>
       </c>
@@ -24080,7 +24080,7 @@
       </c>
     </row>
     <row r="155" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A155" s="125"/>
+      <c r="A155" s="126"/>
       <c r="B155" s="9">
         <v>44</v>
       </c>
@@ -24203,7 +24203,7 @@
       </c>
     </row>
     <row r="156" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A156" s="125"/>
+      <c r="A156" s="126"/>
       <c r="B156" s="9">
         <v>45</v>
       </c>
@@ -24326,7 +24326,7 @@
       </c>
     </row>
     <row r="157" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A157" s="125"/>
+      <c r="A157" s="126"/>
       <c r="B157" s="9">
         <v>46</v>
       </c>
@@ -24449,7 +24449,7 @@
       </c>
     </row>
     <row r="158" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A158" s="125"/>
+      <c r="A158" s="126"/>
       <c r="B158" s="9">
         <v>47</v>
       </c>
@@ -24572,7 +24572,7 @@
       </c>
     </row>
     <row r="159" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A159" s="125"/>
+      <c r="A159" s="126"/>
       <c r="B159" s="9">
         <v>48</v>
       </c>
@@ -24695,7 +24695,7 @@
       </c>
     </row>
     <row r="160" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A160" s="125"/>
+      <c r="A160" s="126"/>
       <c r="B160" s="9">
         <v>49</v>
       </c>
@@ -24818,7 +24818,7 @@
       </c>
     </row>
     <row r="161" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A161" s="125"/>
+      <c r="A161" s="126"/>
       <c r="B161" s="9">
         <v>50</v>
       </c>
@@ -24941,7 +24941,7 @@
       </c>
     </row>
     <row r="162" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A162" s="125"/>
+      <c r="A162" s="126"/>
       <c r="B162" s="9">
         <v>51</v>
       </c>
@@ -25064,7 +25064,7 @@
       </c>
     </row>
     <row r="163" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A163" s="125"/>
+      <c r="A163" s="126"/>
       <c r="B163" s="9">
         <v>52</v>
       </c>
@@ -25187,7 +25187,7 @@
       </c>
     </row>
     <row r="164" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A164" s="125"/>
+      <c r="A164" s="126"/>
       <c r="B164" s="9">
         <v>53</v>
       </c>
@@ -25310,7 +25310,7 @@
       </c>
     </row>
     <row r="165" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A165" s="125"/>
+      <c r="A165" s="126"/>
       <c r="B165" s="9">
         <v>54</v>
       </c>
@@ -25433,7 +25433,7 @@
       </c>
     </row>
     <row r="166" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A166" s="125"/>
+      <c r="A166" s="126"/>
       <c r="B166" s="9">
         <v>55</v>
       </c>
@@ -25556,7 +25556,7 @@
       </c>
     </row>
     <row r="167" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A167" s="125"/>
+      <c r="A167" s="126"/>
       <c r="B167" s="9">
         <v>56</v>
       </c>
@@ -25679,7 +25679,7 @@
       </c>
     </row>
     <row r="168" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A168" s="125"/>
+      <c r="A168" s="126"/>
       <c r="B168" s="9">
         <v>57</v>
       </c>
@@ -25802,7 +25802,7 @@
       </c>
     </row>
     <row r="169" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A169" s="125"/>
+      <c r="A169" s="126"/>
       <c r="B169" s="9">
         <v>58</v>
       </c>
@@ -25925,7 +25925,7 @@
       </c>
     </row>
     <row r="170" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A170" s="125"/>
+      <c r="A170" s="126"/>
       <c r="B170" s="9">
         <v>59</v>
       </c>
@@ -26048,7 +26048,7 @@
       </c>
     </row>
     <row r="171" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A171" s="125"/>
+      <c r="A171" s="126"/>
       <c r="B171" s="9">
         <v>60</v>
       </c>
@@ -26171,7 +26171,7 @@
       </c>
     </row>
     <row r="172" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A172" s="125"/>
+      <c r="A172" s="126"/>
       <c r="B172" s="9">
         <v>61</v>
       </c>
@@ -26294,7 +26294,7 @@
       </c>
     </row>
     <row r="173" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A173" s="125"/>
+      <c r="A173" s="126"/>
       <c r="B173" s="9">
         <v>62</v>
       </c>
@@ -26417,7 +26417,7 @@
       </c>
     </row>
     <row r="174" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A174" s="125"/>
+      <c r="A174" s="126"/>
       <c r="B174" s="9">
         <v>63</v>
       </c>
@@ -26540,7 +26540,7 @@
       </c>
     </row>
     <row r="175" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A175" s="125"/>
+      <c r="A175" s="126"/>
       <c r="B175" s="9">
         <v>64</v>
       </c>
@@ -26663,7 +26663,7 @@
       </c>
     </row>
     <row r="176" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A176" s="125"/>
+      <c r="A176" s="126"/>
       <c r="B176" s="9">
         <v>65</v>
       </c>
@@ -26786,7 +26786,7 @@
       </c>
     </row>
     <row r="177" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A177" s="125"/>
+      <c r="A177" s="126"/>
       <c r="B177" s="9">
         <v>66</v>
       </c>
@@ -26909,7 +26909,7 @@
       </c>
     </row>
     <row r="178" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A178" s="125"/>
+      <c r="A178" s="126"/>
       <c r="B178" s="9">
         <v>67</v>
       </c>
@@ -27032,7 +27032,7 @@
       </c>
     </row>
     <row r="179" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A179" s="125"/>
+      <c r="A179" s="126"/>
       <c r="B179" s="9">
         <v>68</v>
       </c>
@@ -27155,7 +27155,7 @@
       </c>
     </row>
     <row r="180" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A180" s="125"/>
+      <c r="A180" s="126"/>
       <c r="B180" s="9">
         <v>69</v>
       </c>
@@ -27278,7 +27278,7 @@
       </c>
     </row>
     <row r="181" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A181" s="125"/>
+      <c r="A181" s="126"/>
       <c r="B181" s="9">
         <v>70</v>
       </c>
@@ -27401,7 +27401,7 @@
       </c>
     </row>
     <row r="182" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A182" s="125"/>
+      <c r="A182" s="126"/>
       <c r="B182" s="9">
         <v>71</v>
       </c>
@@ -27524,7 +27524,7 @@
       </c>
     </row>
     <row r="183" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A183" s="125"/>
+      <c r="A183" s="126"/>
       <c r="B183" s="9">
         <v>72</v>
       </c>
@@ -27647,7 +27647,7 @@
       </c>
     </row>
     <row r="184" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A184" s="125"/>
+      <c r="A184" s="126"/>
       <c r="B184" s="9">
         <v>73</v>
       </c>
@@ -27770,7 +27770,7 @@
       </c>
     </row>
     <row r="185" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A185" s="125"/>
+      <c r="A185" s="126"/>
       <c r="B185" s="9">
         <v>74</v>
       </c>
@@ -27893,7 +27893,7 @@
       </c>
     </row>
     <row r="186" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A186" s="125"/>
+      <c r="A186" s="126"/>
       <c r="B186" s="9">
         <v>75</v>
       </c>
@@ -28016,7 +28016,7 @@
       </c>
     </row>
     <row r="187" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A187" s="125"/>
+      <c r="A187" s="126"/>
       <c r="B187" s="9">
         <v>76</v>
       </c>
@@ -28139,7 +28139,7 @@
       </c>
     </row>
     <row r="188" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A188" s="125"/>
+      <c r="A188" s="126"/>
       <c r="B188" s="9">
         <v>77</v>
       </c>
@@ -28262,7 +28262,7 @@
       </c>
     </row>
     <row r="189" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A189" s="125"/>
+      <c r="A189" s="126"/>
       <c r="B189" s="9">
         <v>78</v>
       </c>
@@ -28385,7 +28385,7 @@
       </c>
     </row>
     <row r="190" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A190" s="125"/>
+      <c r="A190" s="126"/>
       <c r="B190" s="9">
         <v>79</v>
       </c>
@@ -28508,7 +28508,7 @@
       </c>
     </row>
     <row r="191" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A191" s="125"/>
+      <c r="A191" s="126"/>
       <c r="B191" s="9">
         <v>80</v>
       </c>
@@ -28631,7 +28631,7 @@
       </c>
     </row>
     <row r="192" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A192" s="125"/>
+      <c r="A192" s="126"/>
       <c r="B192" s="9">
         <v>81</v>
       </c>
@@ -28754,7 +28754,7 @@
       </c>
     </row>
     <row r="193" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A193" s="125"/>
+      <c r="A193" s="126"/>
       <c r="B193" s="9">
         <v>82</v>
       </c>
@@ -28877,7 +28877,7 @@
       </c>
     </row>
     <row r="194" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A194" s="125"/>
+      <c r="A194" s="126"/>
       <c r="B194" s="9">
         <v>83</v>
       </c>
@@ -29000,7 +29000,7 @@
       </c>
     </row>
     <row r="195" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A195" s="125"/>
+      <c r="A195" s="126"/>
       <c r="B195" s="9">
         <v>84</v>
       </c>
@@ -29123,7 +29123,7 @@
       </c>
     </row>
     <row r="196" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A196" s="125"/>
+      <c r="A196" s="126"/>
       <c r="B196" s="9">
         <v>85</v>
       </c>
@@ -29246,7 +29246,7 @@
       </c>
     </row>
     <row r="197" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A197" s="125"/>
+      <c r="A197" s="126"/>
       <c r="B197" s="9">
         <v>86</v>
       </c>
@@ -29369,7 +29369,7 @@
       </c>
     </row>
     <row r="198" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A198" s="125"/>
+      <c r="A198" s="126"/>
       <c r="B198" s="9">
         <v>87</v>
       </c>
@@ -29492,7 +29492,7 @@
       </c>
     </row>
     <row r="199" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A199" s="125"/>
+      <c r="A199" s="126"/>
       <c r="B199" s="9">
         <v>88</v>
       </c>
@@ -29615,7 +29615,7 @@
       </c>
     </row>
     <row r="200" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A200" s="125"/>
+      <c r="A200" s="126"/>
       <c r="B200" s="9">
         <v>89</v>
       </c>
@@ -29738,7 +29738,7 @@
       </c>
     </row>
     <row r="201" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A201" s="125"/>
+      <c r="A201" s="126"/>
       <c r="B201" s="9">
         <v>90</v>
       </c>
@@ -29861,7 +29861,7 @@
       </c>
     </row>
     <row r="202" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A202" s="125"/>
+      <c r="A202" s="126"/>
       <c r="B202" s="9">
         <v>91</v>
       </c>
@@ -29984,7 +29984,7 @@
       </c>
     </row>
     <row r="203" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A203" s="125"/>
+      <c r="A203" s="126"/>
       <c r="B203" s="9">
         <v>92</v>
       </c>
@@ -30107,7 +30107,7 @@
       </c>
     </row>
     <row r="204" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A204" s="125"/>
+      <c r="A204" s="126"/>
       <c r="B204" s="9">
         <v>93</v>
       </c>
@@ -30230,7 +30230,7 @@
       </c>
     </row>
     <row r="205" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A205" s="125"/>
+      <c r="A205" s="126"/>
       <c r="B205" s="9">
         <v>94</v>
       </c>
@@ -30353,7 +30353,7 @@
       </c>
     </row>
     <row r="206" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A206" s="125"/>
+      <c r="A206" s="126"/>
       <c r="B206" s="9">
         <v>95</v>
       </c>
@@ -30476,7 +30476,7 @@
       </c>
     </row>
     <row r="207" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A207" s="125"/>
+      <c r="A207" s="126"/>
       <c r="B207" s="9">
         <v>96</v>
       </c>
@@ -30599,7 +30599,7 @@
       </c>
     </row>
     <row r="208" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A208" s="125"/>
+      <c r="A208" s="126"/>
       <c r="B208" s="9">
         <v>97</v>
       </c>
@@ -30722,7 +30722,7 @@
       </c>
     </row>
     <row r="209" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A209" s="125"/>
+      <c r="A209" s="126"/>
       <c r="B209" s="9">
         <v>98</v>
       </c>
@@ -30845,7 +30845,7 @@
       </c>
     </row>
     <row r="210" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A210" s="125"/>
+      <c r="A210" s="126"/>
       <c r="B210" s="9">
         <v>99</v>
       </c>
@@ -30968,7 +30968,7 @@
       </c>
     </row>
     <row r="211" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A211" s="125"/>
+      <c r="A211" s="126"/>
       <c r="B211" s="9" t="s">
         <v>79</v>
       </c>
@@ -31091,7 +31091,7 @@
       </c>
     </row>
     <row r="212" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A212" s="125" t="s">
+      <c r="A212" s="126" t="s">
         <v>51</v>
       </c>
       <c r="B212" s="71" t="s">
@@ -31216,7 +31216,7 @@
       </c>
     </row>
     <row r="213" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A213" s="125"/>
+      <c r="A213" s="126"/>
       <c r="B213" s="9">
         <v>0</v>
       </c>
@@ -31339,7 +31339,7 @@
       </c>
     </row>
     <row r="214" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A214" s="125"/>
+      <c r="A214" s="126"/>
       <c r="B214" s="9">
         <v>1</v>
       </c>
@@ -31462,7 +31462,7 @@
       </c>
     </row>
     <row r="215" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A215" s="125"/>
+      <c r="A215" s="126"/>
       <c r="B215" s="9">
         <v>2</v>
       </c>
@@ -31585,7 +31585,7 @@
       </c>
     </row>
     <row r="216" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A216" s="125"/>
+      <c r="A216" s="126"/>
       <c r="B216" s="9">
         <v>3</v>
       </c>
@@ -31708,7 +31708,7 @@
       </c>
     </row>
     <row r="217" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A217" s="125"/>
+      <c r="A217" s="126"/>
       <c r="B217" s="9">
         <v>4</v>
       </c>
@@ -31831,7 +31831,7 @@
       </c>
     </row>
     <row r="218" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A218" s="125"/>
+      <c r="A218" s="126"/>
       <c r="B218" s="9">
         <v>5</v>
       </c>
@@ -31954,7 +31954,7 @@
       </c>
     </row>
     <row r="219" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A219" s="125"/>
+      <c r="A219" s="126"/>
       <c r="B219" s="9">
         <v>6</v>
       </c>
@@ -32077,7 +32077,7 @@
       </c>
     </row>
     <row r="220" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A220" s="125"/>
+      <c r="A220" s="126"/>
       <c r="B220" s="9">
         <v>7</v>
       </c>
@@ -32200,7 +32200,7 @@
       </c>
     </row>
     <row r="221" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A221" s="125"/>
+      <c r="A221" s="126"/>
       <c r="B221" s="9">
         <v>8</v>
       </c>
@@ -32323,7 +32323,7 @@
       </c>
     </row>
     <row r="222" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A222" s="125"/>
+      <c r="A222" s="126"/>
       <c r="B222" s="9">
         <v>9</v>
       </c>
@@ -32446,7 +32446,7 @@
       </c>
     </row>
     <row r="223" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A223" s="125"/>
+      <c r="A223" s="126"/>
       <c r="B223" s="9">
         <v>10</v>
       </c>
@@ -32569,7 +32569,7 @@
       </c>
     </row>
     <row r="224" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A224" s="125"/>
+      <c r="A224" s="126"/>
       <c r="B224" s="9">
         <v>11</v>
       </c>
@@ -32692,7 +32692,7 @@
       </c>
     </row>
     <row r="225" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A225" s="125"/>
+      <c r="A225" s="126"/>
       <c r="B225" s="9">
         <v>12</v>
       </c>
@@ -32815,7 +32815,7 @@
       </c>
     </row>
     <row r="226" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A226" s="125"/>
+      <c r="A226" s="126"/>
       <c r="B226" s="9">
         <v>13</v>
       </c>
@@ -32938,7 +32938,7 @@
       </c>
     </row>
     <row r="227" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A227" s="125"/>
+      <c r="A227" s="126"/>
       <c r="B227" s="9">
         <v>14</v>
       </c>
@@ -33061,7 +33061,7 @@
       </c>
     </row>
     <row r="228" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A228" s="125"/>
+      <c r="A228" s="126"/>
       <c r="B228" s="9">
         <v>15</v>
       </c>
@@ -33184,7 +33184,7 @@
       </c>
     </row>
     <row r="229" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A229" s="125"/>
+      <c r="A229" s="126"/>
       <c r="B229" s="9">
         <v>16</v>
       </c>
@@ -33307,7 +33307,7 @@
       </c>
     </row>
     <row r="230" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A230" s="125"/>
+      <c r="A230" s="126"/>
       <c r="B230" s="9">
         <v>17</v>
       </c>
@@ -33430,7 +33430,7 @@
       </c>
     </row>
     <row r="231" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A231" s="125"/>
+      <c r="A231" s="126"/>
       <c r="B231" s="9">
         <v>18</v>
       </c>
@@ -33553,7 +33553,7 @@
       </c>
     </row>
     <row r="232" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A232" s="125"/>
+      <c r="A232" s="126"/>
       <c r="B232" s="9">
         <v>19</v>
       </c>
@@ -33676,7 +33676,7 @@
       </c>
     </row>
     <row r="233" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A233" s="125"/>
+      <c r="A233" s="126"/>
       <c r="B233" s="9">
         <v>20</v>
       </c>
@@ -33799,7 +33799,7 @@
       </c>
     </row>
     <row r="234" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A234" s="125"/>
+      <c r="A234" s="126"/>
       <c r="B234" s="9">
         <v>21</v>
       </c>
@@ -33922,7 +33922,7 @@
       </c>
     </row>
     <row r="235" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A235" s="125"/>
+      <c r="A235" s="126"/>
       <c r="B235" s="9">
         <v>22</v>
       </c>
@@ -34045,7 +34045,7 @@
       </c>
     </row>
     <row r="236" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A236" s="125"/>
+      <c r="A236" s="126"/>
       <c r="B236" s="9">
         <v>23</v>
       </c>
@@ -34168,7 +34168,7 @@
       </c>
     </row>
     <row r="237" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A237" s="125"/>
+      <c r="A237" s="126"/>
       <c r="B237" s="9">
         <v>24</v>
       </c>
@@ -34291,7 +34291,7 @@
       </c>
     </row>
     <row r="238" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A238" s="125"/>
+      <c r="A238" s="126"/>
       <c r="B238" s="9">
         <v>25</v>
       </c>
@@ -34414,7 +34414,7 @@
       </c>
     </row>
     <row r="239" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A239" s="125"/>
+      <c r="A239" s="126"/>
       <c r="B239" s="9">
         <v>26</v>
       </c>
@@ -34537,7 +34537,7 @@
       </c>
     </row>
     <row r="240" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A240" s="125"/>
+      <c r="A240" s="126"/>
       <c r="B240" s="9">
         <v>27</v>
       </c>
@@ -34660,7 +34660,7 @@
       </c>
     </row>
     <row r="241" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A241" s="125"/>
+      <c r="A241" s="126"/>
       <c r="B241" s="9">
         <v>28</v>
       </c>
@@ -34783,7 +34783,7 @@
       </c>
     </row>
     <row r="242" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A242" s="125"/>
+      <c r="A242" s="126"/>
       <c r="B242" s="9">
         <v>29</v>
       </c>
@@ -34906,7 +34906,7 @@
       </c>
     </row>
     <row r="243" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A243" s="125"/>
+      <c r="A243" s="126"/>
       <c r="B243" s="9">
         <v>30</v>
       </c>
@@ -35029,7 +35029,7 @@
       </c>
     </row>
     <row r="244" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A244" s="125"/>
+      <c r="A244" s="126"/>
       <c r="B244" s="9">
         <v>31</v>
       </c>
@@ -35152,7 +35152,7 @@
       </c>
     </row>
     <row r="245" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A245" s="125"/>
+      <c r="A245" s="126"/>
       <c r="B245" s="9">
         <v>32</v>
       </c>
@@ -35275,7 +35275,7 @@
       </c>
     </row>
     <row r="246" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A246" s="125"/>
+      <c r="A246" s="126"/>
       <c r="B246" s="9">
         <v>33</v>
       </c>
@@ -35398,7 +35398,7 @@
       </c>
     </row>
     <row r="247" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A247" s="125"/>
+      <c r="A247" s="126"/>
       <c r="B247" s="9">
         <v>34</v>
       </c>
@@ -35521,7 +35521,7 @@
       </c>
     </row>
     <row r="248" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A248" s="125"/>
+      <c r="A248" s="126"/>
       <c r="B248" s="9">
         <v>35</v>
       </c>
@@ -35644,7 +35644,7 @@
       </c>
     </row>
     <row r="249" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A249" s="125"/>
+      <c r="A249" s="126"/>
       <c r="B249" s="9">
         <v>36</v>
       </c>
@@ -35767,7 +35767,7 @@
       </c>
     </row>
     <row r="250" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A250" s="125"/>
+      <c r="A250" s="126"/>
       <c r="B250" s="9">
         <v>37</v>
       </c>
@@ -35890,7 +35890,7 @@
       </c>
     </row>
     <row r="251" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A251" s="125"/>
+      <c r="A251" s="126"/>
       <c r="B251" s="9">
         <v>38</v>
       </c>
@@ -36013,7 +36013,7 @@
       </c>
     </row>
     <row r="252" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A252" s="125"/>
+      <c r="A252" s="126"/>
       <c r="B252" s="9">
         <v>39</v>
       </c>
@@ -36136,7 +36136,7 @@
       </c>
     </row>
     <row r="253" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A253" s="125"/>
+      <c r="A253" s="126"/>
       <c r="B253" s="9">
         <v>40</v>
       </c>
@@ -36259,7 +36259,7 @@
       </c>
     </row>
     <row r="254" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A254" s="125"/>
+      <c r="A254" s="126"/>
       <c r="B254" s="9">
         <v>41</v>
       </c>
@@ -36382,7 +36382,7 @@
       </c>
     </row>
     <row r="255" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A255" s="125"/>
+      <c r="A255" s="126"/>
       <c r="B255" s="9">
         <v>42</v>
       </c>
@@ -36505,7 +36505,7 @@
       </c>
     </row>
     <row r="256" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A256" s="125"/>
+      <c r="A256" s="126"/>
       <c r="B256" s="9">
         <v>43</v>
       </c>
@@ -36628,7 +36628,7 @@
       </c>
     </row>
     <row r="257" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A257" s="125"/>
+      <c r="A257" s="126"/>
       <c r="B257" s="9">
         <v>44</v>
       </c>
@@ -36751,7 +36751,7 @@
       </c>
     </row>
     <row r="258" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A258" s="125"/>
+      <c r="A258" s="126"/>
       <c r="B258" s="9">
         <v>45</v>
       </c>
@@ -36874,7 +36874,7 @@
       </c>
     </row>
     <row r="259" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A259" s="125"/>
+      <c r="A259" s="126"/>
       <c r="B259" s="9">
         <v>46</v>
       </c>
@@ -36997,7 +36997,7 @@
       </c>
     </row>
     <row r="260" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A260" s="125"/>
+      <c r="A260" s="126"/>
       <c r="B260" s="9">
         <v>47</v>
       </c>
@@ -37120,7 +37120,7 @@
       </c>
     </row>
     <row r="261" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A261" s="125"/>
+      <c r="A261" s="126"/>
       <c r="B261" s="9">
         <v>48</v>
       </c>
@@ -37243,7 +37243,7 @@
       </c>
     </row>
     <row r="262" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A262" s="125"/>
+      <c r="A262" s="126"/>
       <c r="B262" s="9">
         <v>49</v>
       </c>
@@ -37366,7 +37366,7 @@
       </c>
     </row>
     <row r="263" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A263" s="125"/>
+      <c r="A263" s="126"/>
       <c r="B263" s="9">
         <v>50</v>
       </c>
@@ -37489,7 +37489,7 @@
       </c>
     </row>
     <row r="264" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A264" s="125"/>
+      <c r="A264" s="126"/>
       <c r="B264" s="9">
         <v>51</v>
       </c>
@@ -37612,7 +37612,7 @@
       </c>
     </row>
     <row r="265" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A265" s="125"/>
+      <c r="A265" s="126"/>
       <c r="B265" s="9">
         <v>52</v>
       </c>
@@ -37735,7 +37735,7 @@
       </c>
     </row>
     <row r="266" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A266" s="125"/>
+      <c r="A266" s="126"/>
       <c r="B266" s="9">
         <v>53</v>
       </c>
@@ -37858,7 +37858,7 @@
       </c>
     </row>
     <row r="267" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A267" s="125"/>
+      <c r="A267" s="126"/>
       <c r="B267" s="9">
         <v>54</v>
       </c>
@@ -37981,7 +37981,7 @@
       </c>
     </row>
     <row r="268" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A268" s="125"/>
+      <c r="A268" s="126"/>
       <c r="B268" s="9">
         <v>55</v>
       </c>
@@ -38104,7 +38104,7 @@
       </c>
     </row>
     <row r="269" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A269" s="125"/>
+      <c r="A269" s="126"/>
       <c r="B269" s="9">
         <v>56</v>
       </c>
@@ -38227,7 +38227,7 @@
       </c>
     </row>
     <row r="270" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A270" s="125"/>
+      <c r="A270" s="126"/>
       <c r="B270" s="9">
         <v>57</v>
       </c>
@@ -38350,7 +38350,7 @@
       </c>
     </row>
     <row r="271" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A271" s="125"/>
+      <c r="A271" s="126"/>
       <c r="B271" s="9">
         <v>58</v>
       </c>
@@ -38473,7 +38473,7 @@
       </c>
     </row>
     <row r="272" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A272" s="125"/>
+      <c r="A272" s="126"/>
       <c r="B272" s="9">
         <v>59</v>
       </c>
@@ -38596,7 +38596,7 @@
       </c>
     </row>
     <row r="273" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A273" s="125"/>
+      <c r="A273" s="126"/>
       <c r="B273" s="9">
         <v>60</v>
       </c>
@@ -38719,7 +38719,7 @@
       </c>
     </row>
     <row r="274" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A274" s="125"/>
+      <c r="A274" s="126"/>
       <c r="B274" s="9">
         <v>61</v>
       </c>
@@ -38842,7 +38842,7 @@
       </c>
     </row>
     <row r="275" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A275" s="125"/>
+      <c r="A275" s="126"/>
       <c r="B275" s="9">
         <v>62</v>
       </c>
@@ -38965,7 +38965,7 @@
       </c>
     </row>
     <row r="276" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A276" s="125"/>
+      <c r="A276" s="126"/>
       <c r="B276" s="9">
         <v>63</v>
       </c>
@@ -39088,7 +39088,7 @@
       </c>
     </row>
     <row r="277" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A277" s="125"/>
+      <c r="A277" s="126"/>
       <c r="B277" s="9">
         <v>64</v>
       </c>
@@ -39211,7 +39211,7 @@
       </c>
     </row>
     <row r="278" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A278" s="125"/>
+      <c r="A278" s="126"/>
       <c r="B278" s="9">
         <v>65</v>
       </c>
@@ -39334,7 +39334,7 @@
       </c>
     </row>
     <row r="279" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A279" s="125"/>
+      <c r="A279" s="126"/>
       <c r="B279" s="9">
         <v>66</v>
       </c>
@@ -39457,7 +39457,7 @@
       </c>
     </row>
     <row r="280" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A280" s="125"/>
+      <c r="A280" s="126"/>
       <c r="B280" s="9">
         <v>67</v>
       </c>
@@ -39580,7 +39580,7 @@
       </c>
     </row>
     <row r="281" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A281" s="125"/>
+      <c r="A281" s="126"/>
       <c r="B281" s="9">
         <v>68</v>
       </c>
@@ -39703,7 +39703,7 @@
       </c>
     </row>
     <row r="282" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A282" s="125"/>
+      <c r="A282" s="126"/>
       <c r="B282" s="9">
         <v>69</v>
       </c>
@@ -39826,7 +39826,7 @@
       </c>
     </row>
     <row r="283" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A283" s="125"/>
+      <c r="A283" s="126"/>
       <c r="B283" s="9">
         <v>70</v>
       </c>
@@ -39949,7 +39949,7 @@
       </c>
     </row>
     <row r="284" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A284" s="125"/>
+      <c r="A284" s="126"/>
       <c r="B284" s="9">
         <v>71</v>
       </c>
@@ -40072,7 +40072,7 @@
       </c>
     </row>
     <row r="285" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A285" s="125"/>
+      <c r="A285" s="126"/>
       <c r="B285" s="9">
         <v>72</v>
       </c>
@@ -40195,7 +40195,7 @@
       </c>
     </row>
     <row r="286" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A286" s="125"/>
+      <c r="A286" s="126"/>
       <c r="B286" s="9">
         <v>73</v>
       </c>
@@ -40318,7 +40318,7 @@
       </c>
     </row>
     <row r="287" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A287" s="125"/>
+      <c r="A287" s="126"/>
       <c r="B287" s="9">
         <v>74</v>
       </c>
@@ -40441,7 +40441,7 @@
       </c>
     </row>
     <row r="288" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A288" s="125"/>
+      <c r="A288" s="126"/>
       <c r="B288" s="9">
         <v>75</v>
       </c>
@@ -40564,7 +40564,7 @@
       </c>
     </row>
     <row r="289" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A289" s="125"/>
+      <c r="A289" s="126"/>
       <c r="B289" s="9">
         <v>76</v>
       </c>
@@ -40687,7 +40687,7 @@
       </c>
     </row>
     <row r="290" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A290" s="125"/>
+      <c r="A290" s="126"/>
       <c r="B290" s="9">
         <v>77</v>
       </c>
@@ -40810,7 +40810,7 @@
       </c>
     </row>
     <row r="291" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A291" s="125"/>
+      <c r="A291" s="126"/>
       <c r="B291" s="9">
         <v>78</v>
       </c>
@@ -40933,7 +40933,7 @@
       </c>
     </row>
     <row r="292" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A292" s="125"/>
+      <c r="A292" s="126"/>
       <c r="B292" s="9">
         <v>79</v>
       </c>
@@ -41056,7 +41056,7 @@
       </c>
     </row>
     <row r="293" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A293" s="125"/>
+      <c r="A293" s="126"/>
       <c r="B293" s="9">
         <v>80</v>
       </c>
@@ -41179,7 +41179,7 @@
       </c>
     </row>
     <row r="294" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A294" s="125"/>
+      <c r="A294" s="126"/>
       <c r="B294" s="9">
         <v>81</v>
       </c>
@@ -41302,7 +41302,7 @@
       </c>
     </row>
     <row r="295" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A295" s="125"/>
+      <c r="A295" s="126"/>
       <c r="B295" s="9">
         <v>82</v>
       </c>
@@ -41425,7 +41425,7 @@
       </c>
     </row>
     <row r="296" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A296" s="125"/>
+      <c r="A296" s="126"/>
       <c r="B296" s="9">
         <v>83</v>
       </c>
@@ -41548,7 +41548,7 @@
       </c>
     </row>
     <row r="297" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A297" s="125"/>
+      <c r="A297" s="126"/>
       <c r="B297" s="9">
         <v>84</v>
       </c>
@@ -41671,7 +41671,7 @@
       </c>
     </row>
     <row r="298" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A298" s="125"/>
+      <c r="A298" s="126"/>
       <c r="B298" s="9">
         <v>85</v>
       </c>
@@ -41794,7 +41794,7 @@
       </c>
     </row>
     <row r="299" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A299" s="125"/>
+      <c r="A299" s="126"/>
       <c r="B299" s="9">
         <v>86</v>
       </c>
@@ -41917,7 +41917,7 @@
       </c>
     </row>
     <row r="300" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A300" s="125"/>
+      <c r="A300" s="126"/>
       <c r="B300" s="9">
         <v>87</v>
       </c>
@@ -42040,7 +42040,7 @@
       </c>
     </row>
     <row r="301" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A301" s="125"/>
+      <c r="A301" s="126"/>
       <c r="B301" s="9">
         <v>88</v>
       </c>
@@ -42163,7 +42163,7 @@
       </c>
     </row>
     <row r="302" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A302" s="125"/>
+      <c r="A302" s="126"/>
       <c r="B302" s="9">
         <v>89</v>
       </c>
@@ -42286,7 +42286,7 @@
       </c>
     </row>
     <row r="303" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A303" s="125"/>
+      <c r="A303" s="126"/>
       <c r="B303" s="9">
         <v>90</v>
       </c>
@@ -42409,7 +42409,7 @@
       </c>
     </row>
     <row r="304" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A304" s="125"/>
+      <c r="A304" s="126"/>
       <c r="B304" s="9">
         <v>91</v>
       </c>
@@ -42532,7 +42532,7 @@
       </c>
     </row>
     <row r="305" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A305" s="125"/>
+      <c r="A305" s="126"/>
       <c r="B305" s="9">
         <v>92</v>
       </c>
@@ -42655,7 +42655,7 @@
       </c>
     </row>
     <row r="306" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A306" s="125"/>
+      <c r="A306" s="126"/>
       <c r="B306" s="9">
         <v>93</v>
       </c>
@@ -42778,7 +42778,7 @@
       </c>
     </row>
     <row r="307" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A307" s="125"/>
+      <c r="A307" s="126"/>
       <c r="B307" s="9">
         <v>94</v>
       </c>
@@ -42901,7 +42901,7 @@
       </c>
     </row>
     <row r="308" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A308" s="125"/>
+      <c r="A308" s="126"/>
       <c r="B308" s="9">
         <v>95</v>
       </c>
@@ -43024,7 +43024,7 @@
       </c>
     </row>
     <row r="309" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A309" s="125"/>
+      <c r="A309" s="126"/>
       <c r="B309" s="9">
         <v>96</v>
       </c>
@@ -43147,7 +43147,7 @@
       </c>
     </row>
     <row r="310" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A310" s="125"/>
+      <c r="A310" s="126"/>
       <c r="B310" s="9">
         <v>97</v>
       </c>
@@ -43270,7 +43270,7 @@
       </c>
     </row>
     <row r="311" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A311" s="125"/>
+      <c r="A311" s="126"/>
       <c r="B311" s="9">
         <v>98</v>
       </c>
@@ -43393,7 +43393,7 @@
       </c>
     </row>
     <row r="312" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A312" s="125"/>
+      <c r="A312" s="126"/>
       <c r="B312" s="9">
         <v>99</v>
       </c>
@@ -43516,7 +43516,7 @@
       </c>
     </row>
     <row r="313" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A313" s="125"/>
+      <c r="A313" s="126"/>
       <c r="B313" s="10" t="s">
         <v>79</v>
       </c>
@@ -43636,6 +43636,12 @@
       </c>
       <c r="AO313" s="4">
         <v>4147</v>
+      </c>
+    </row>
+    <row r="333" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H333" s="122">
+        <f>SUM(L8:AO8)/30</f>
+        <v>3279110.2</v>
       </c>
     </row>
   </sheetData>
@@ -43677,8 +43683,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="132"/>
-      <c r="B1" s="132"/>
+      <c r="A1" s="133"/>
+      <c r="B1" s="133"/>
       <c r="C1" s="63" t="s">
         <v>54</v>
       </c>
@@ -43722,10 +43728,10 @@
       <c r="AO1" s="64"/>
     </row>
     <row r="2" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="127"/>
+      <c r="B2" s="128"/>
       <c r="D2" s="26" t="s">
         <v>40</v>
       </c>
@@ -43768,10 +43774,10 @@
       <c r="AO2" s="28"/>
     </row>
     <row r="3" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="128"/>
+      <c r="B3" s="129"/>
       <c r="D3" s="19" t="s">
         <v>69</v>
       </c>
@@ -44075,7 +44081,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="130" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="69" t="s">
@@ -44200,7 +44206,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A9" s="130"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="52" t="s">
         <v>20</v>
       </c>
@@ -44323,7 +44329,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" s="130"/>
+      <c r="A10" s="131"/>
       <c r="B10" s="52" t="s">
         <v>21</v>
       </c>
@@ -44446,7 +44452,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A11" s="130"/>
+      <c r="A11" s="131"/>
       <c r="B11" s="53" t="s">
         <v>22</v>
       </c>
@@ -44569,7 +44575,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" s="130"/>
+      <c r="A12" s="131"/>
       <c r="B12" s="52" t="s">
         <v>23</v>
       </c>
@@ -44692,7 +44698,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="130"/>
+      <c r="A13" s="131"/>
       <c r="B13" s="52" t="s">
         <v>24</v>
       </c>
@@ -44815,7 +44821,7 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" s="130"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="52" t="s">
         <v>25</v>
       </c>
@@ -44938,7 +44944,7 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A15" s="130"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="52" t="s">
         <v>26</v>
       </c>
@@ -45061,7 +45067,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" s="130"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="52" t="s">
         <v>27</v>
       </c>
@@ -45184,7 +45190,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A17" s="130"/>
+      <c r="A17" s="131"/>
       <c r="B17" s="52" t="s">
         <v>28</v>
       </c>
@@ -45307,7 +45313,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A18" s="130"/>
+      <c r="A18" s="131"/>
       <c r="B18" s="52" t="s">
         <v>29</v>
       </c>
@@ -45430,7 +45436,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A19" s="130"/>
+      <c r="A19" s="131"/>
       <c r="B19" s="52" t="s">
         <v>30</v>
       </c>
@@ -45553,7 +45559,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A20" s="130"/>
+      <c r="A20" s="131"/>
       <c r="B20" s="52" t="s">
         <v>31</v>
       </c>
@@ -45676,7 +45682,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A21" s="130"/>
+      <c r="A21" s="131"/>
       <c r="B21" s="52" t="s">
         <v>32</v>
       </c>
@@ -45799,7 +45805,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A22" s="130"/>
+      <c r="A22" s="131"/>
       <c r="B22" s="53" t="s">
         <v>33</v>
       </c>
@@ -45922,7 +45928,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A23" s="130"/>
+      <c r="A23" s="131"/>
       <c r="B23" s="52" t="s">
         <v>34</v>
       </c>
@@ -46045,7 +46051,7 @@
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A24" s="130"/>
+      <c r="A24" s="131"/>
       <c r="B24" s="52" t="s">
         <v>35</v>
       </c>
@@ -46168,7 +46174,7 @@
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A25" s="130"/>
+      <c r="A25" s="131"/>
       <c r="B25" s="52" t="s">
         <v>36</v>
       </c>
@@ -46291,7 +46297,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A26" s="130"/>
+      <c r="A26" s="131"/>
       <c r="B26" s="52" t="s">
         <v>37</v>
       </c>
@@ -46414,7 +46420,7 @@
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A27" s="130"/>
+      <c r="A27" s="131"/>
       <c r="B27" s="62" t="s">
         <v>80</v>
       </c>
@@ -46537,7 +46543,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A28" s="130"/>
+      <c r="A28" s="131"/>
       <c r="B28" s="62" t="s">
         <v>81</v>
       </c>
@@ -46660,7 +46666,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A29" s="131"/>
+      <c r="A29" s="132"/>
       <c r="B29" s="54" t="s">
         <v>79</v>
       </c>
@@ -46783,7 +46789,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A30" s="130" t="s">
+      <c r="A30" s="131" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="69" t="s">
@@ -46908,7 +46914,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A31" s="130"/>
+      <c r="A31" s="131"/>
       <c r="B31" s="52" t="s">
         <v>20</v>
       </c>
@@ -47031,7 +47037,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A32" s="130"/>
+      <c r="A32" s="131"/>
       <c r="B32" s="52" t="s">
         <v>21</v>
       </c>
@@ -47154,7 +47160,7 @@
       </c>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A33" s="130"/>
+      <c r="A33" s="131"/>
       <c r="B33" s="52" t="s">
         <v>22</v>
       </c>
@@ -47277,7 +47283,7 @@
       </c>
     </row>
     <row r="34" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A34" s="130"/>
+      <c r="A34" s="131"/>
       <c r="B34" s="52" t="s">
         <v>23</v>
       </c>
@@ -47400,7 +47406,7 @@
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A35" s="130"/>
+      <c r="A35" s="131"/>
       <c r="B35" s="52" t="s">
         <v>24</v>
       </c>
@@ -47523,7 +47529,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A36" s="130"/>
+      <c r="A36" s="131"/>
       <c r="B36" s="52" t="s">
         <v>25</v>
       </c>
@@ -47646,7 +47652,7 @@
       </c>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A37" s="130"/>
+      <c r="A37" s="131"/>
       <c r="B37" s="52" t="s">
         <v>26</v>
       </c>
@@ -47769,7 +47775,7 @@
       </c>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A38" s="130"/>
+      <c r="A38" s="131"/>
       <c r="B38" s="52" t="s">
         <v>27</v>
       </c>
@@ -47892,7 +47898,7 @@
       </c>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A39" s="130"/>
+      <c r="A39" s="131"/>
       <c r="B39" s="52" t="s">
         <v>28</v>
       </c>
@@ -48015,7 +48021,7 @@
       </c>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A40" s="130"/>
+      <c r="A40" s="131"/>
       <c r="B40" s="52" t="s">
         <v>29</v>
       </c>
@@ -48138,7 +48144,7 @@
       </c>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A41" s="130"/>
+      <c r="A41" s="131"/>
       <c r="B41" s="52" t="s">
         <v>30</v>
       </c>
@@ -48261,7 +48267,7 @@
       </c>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A42" s="130"/>
+      <c r="A42" s="131"/>
       <c r="B42" s="52" t="s">
         <v>31</v>
       </c>
@@ -48384,7 +48390,7 @@
       </c>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A43" s="130"/>
+      <c r="A43" s="131"/>
       <c r="B43" s="52" t="s">
         <v>32</v>
       </c>
@@ -48507,7 +48513,7 @@
       </c>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A44" s="130"/>
+      <c r="A44" s="131"/>
       <c r="B44" s="53" t="s">
         <v>33</v>
       </c>
@@ -48630,7 +48636,7 @@
       </c>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A45" s="130"/>
+      <c r="A45" s="131"/>
       <c r="B45" s="52" t="s">
         <v>34</v>
       </c>
@@ -48753,7 +48759,7 @@
       </c>
     </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A46" s="130"/>
+      <c r="A46" s="131"/>
       <c r="B46" s="52" t="s">
         <v>35</v>
       </c>
@@ -48876,7 +48882,7 @@
       </c>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A47" s="130"/>
+      <c r="A47" s="131"/>
       <c r="B47" s="52" t="s">
         <v>36</v>
       </c>
@@ -48999,7 +49005,7 @@
       </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A48" s="130"/>
+      <c r="A48" s="131"/>
       <c r="B48" s="52" t="s">
         <v>37</v>
       </c>
@@ -49122,7 +49128,7 @@
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A49" s="130"/>
+      <c r="A49" s="131"/>
       <c r="B49" s="62" t="s">
         <v>80</v>
       </c>
@@ -49245,7 +49251,7 @@
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A50" s="130"/>
+      <c r="A50" s="131"/>
       <c r="B50" s="62" t="s">
         <v>81</v>
       </c>
@@ -49368,7 +49374,7 @@
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A51" s="130"/>
+      <c r="A51" s="131"/>
       <c r="B51" s="54" t="s">
         <v>79</v>
       </c>
@@ -49491,7 +49497,7 @@
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A52" s="129" t="s">
+      <c r="A52" s="130" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="69" t="s">
@@ -49616,7 +49622,7 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A53" s="130"/>
+      <c r="A53" s="131"/>
       <c r="B53" s="52" t="s">
         <v>20</v>
       </c>
@@ -49739,7 +49745,7 @@
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A54" s="130"/>
+      <c r="A54" s="131"/>
       <c r="B54" s="52" t="s">
         <v>21</v>
       </c>
@@ -49862,7 +49868,7 @@
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A55" s="130"/>
+      <c r="A55" s="131"/>
       <c r="B55" s="52" t="s">
         <v>22</v>
       </c>
@@ -49985,7 +49991,7 @@
       </c>
     </row>
     <row r="56" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A56" s="130"/>
+      <c r="A56" s="131"/>
       <c r="B56" s="52" t="s">
         <v>23</v>
       </c>
@@ -50108,7 +50114,7 @@
       </c>
     </row>
     <row r="57" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A57" s="130"/>
+      <c r="A57" s="131"/>
       <c r="B57" s="52" t="s">
         <v>24</v>
       </c>
@@ -50231,7 +50237,7 @@
       </c>
     </row>
     <row r="58" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A58" s="130"/>
+      <c r="A58" s="131"/>
       <c r="B58" s="52" t="s">
         <v>25</v>
       </c>
@@ -50354,7 +50360,7 @@
       </c>
     </row>
     <row r="59" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A59" s="130"/>
+      <c r="A59" s="131"/>
       <c r="B59" s="52" t="s">
         <v>26</v>
       </c>
@@ -50477,7 +50483,7 @@
       </c>
     </row>
     <row r="60" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A60" s="130"/>
+      <c r="A60" s="131"/>
       <c r="B60" s="52" t="s">
         <v>27</v>
       </c>
@@ -50600,7 +50606,7 @@
       </c>
     </row>
     <row r="61" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A61" s="130"/>
+      <c r="A61" s="131"/>
       <c r="B61" s="52" t="s">
         <v>28</v>
       </c>
@@ -50723,7 +50729,7 @@
       </c>
     </row>
     <row r="62" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A62" s="130"/>
+      <c r="A62" s="131"/>
       <c r="B62" s="52" t="s">
         <v>29</v>
       </c>
@@ -50846,7 +50852,7 @@
       </c>
     </row>
     <row r="63" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A63" s="130"/>
+      <c r="A63" s="131"/>
       <c r="B63" s="52" t="s">
         <v>30</v>
       </c>
@@ -50969,7 +50975,7 @@
       </c>
     </row>
     <row r="64" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A64" s="130"/>
+      <c r="A64" s="131"/>
       <c r="B64" s="52" t="s">
         <v>31</v>
       </c>
@@ -51092,7 +51098,7 @@
       </c>
     </row>
     <row r="65" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A65" s="130"/>
+      <c r="A65" s="131"/>
       <c r="B65" s="52" t="s">
         <v>32</v>
       </c>
@@ -51215,7 +51221,7 @@
       </c>
     </row>
     <row r="66" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A66" s="130"/>
+      <c r="A66" s="131"/>
       <c r="B66" s="53" t="s">
         <v>33</v>
       </c>
@@ -51338,7 +51344,7 @@
       </c>
     </row>
     <row r="67" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A67" s="130"/>
+      <c r="A67" s="131"/>
       <c r="B67" s="52" t="s">
         <v>34</v>
       </c>
@@ -51461,7 +51467,7 @@
       </c>
     </row>
     <row r="68" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A68" s="130"/>
+      <c r="A68" s="131"/>
       <c r="B68" s="52" t="s">
         <v>35</v>
       </c>
@@ -51584,7 +51590,7 @@
       </c>
     </row>
     <row r="69" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A69" s="130"/>
+      <c r="A69" s="131"/>
       <c r="B69" s="52" t="s">
         <v>36</v>
       </c>
@@ -51707,7 +51713,7 @@
       </c>
     </row>
     <row r="70" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A70" s="130"/>
+      <c r="A70" s="131"/>
       <c r="B70" s="52" t="s">
         <v>37</v>
       </c>
@@ -51830,7 +51836,7 @@
       </c>
     </row>
     <row r="71" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A71" s="130"/>
+      <c r="A71" s="131"/>
       <c r="B71" s="52" t="s">
         <v>80</v>
       </c>
@@ -51953,7 +51959,7 @@
       </c>
     </row>
     <row r="72" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A72" s="130"/>
+      <c r="A72" s="131"/>
       <c r="B72" s="62" t="s">
         <v>81</v>
       </c>
@@ -52076,7 +52082,7 @@
       </c>
     </row>
     <row r="73" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A73" s="131"/>
+      <c r="A73" s="132"/>
       <c r="B73" s="54" t="s">
         <v>79</v>
       </c>
@@ -52242,8 +52248,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="136"/>
-      <c r="B1" s="136"/>
+      <c r="A1" s="137"/>
+      <c r="B1" s="137"/>
       <c r="C1" s="65" t="s">
         <v>67</v>
       </c>
@@ -52287,10 +52293,10 @@
       <c r="AO1" s="64"/>
     </row>
     <row r="2" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="127"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="29"/>
       <c r="D2" s="26" t="s">
         <v>40</v>
@@ -52334,10 +52340,10 @@
       <c r="AO2" s="24"/>
     </row>
     <row r="3" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="128"/>
+      <c r="B3" s="129"/>
       <c r="D3" s="19" t="s">
         <v>68</v>
       </c>
@@ -52639,7 +52645,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" s="133" t="s">
+      <c r="A8" s="134" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="69" t="s">
@@ -52764,7 +52770,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A9" s="134"/>
+      <c r="A9" s="135"/>
       <c r="B9" s="52" t="s">
         <v>8</v>
       </c>
@@ -52887,7 +52893,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" s="134"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="52" t="s">
         <v>9</v>
       </c>
@@ -53010,7 +53016,7 @@
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A11" s="134"/>
+      <c r="A11" s="135"/>
       <c r="B11" s="52" t="s">
         <v>11</v>
       </c>
@@ -53133,7 +53139,7 @@
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" s="134"/>
+      <c r="A12" s="135"/>
       <c r="B12" s="52" t="s">
         <v>12</v>
       </c>
@@ -53256,7 +53262,7 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="134"/>
+      <c r="A13" s="135"/>
       <c r="B13" s="52" t="s">
         <v>10</v>
       </c>
@@ -53379,7 +53385,7 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" s="134"/>
+      <c r="A14" s="135"/>
       <c r="B14" s="52" t="s">
         <v>0</v>
       </c>
@@ -53502,7 +53508,7 @@
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A15" s="134"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="52" t="s">
         <v>1</v>
       </c>
@@ -53625,7 +53631,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" s="134"/>
+      <c r="A16" s="135"/>
       <c r="B16" s="53" t="s">
         <v>18</v>
       </c>
@@ -53748,7 +53754,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A17" s="134"/>
+      <c r="A17" s="135"/>
       <c r="B17" s="52" t="s">
         <v>19</v>
       </c>
@@ -53871,7 +53877,7 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A18" s="134"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="52" t="s">
         <v>2</v>
       </c>
@@ -53994,7 +54000,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A19" s="134"/>
+      <c r="A19" s="135"/>
       <c r="B19" s="52" t="s">
         <v>3</v>
       </c>
@@ -54117,7 +54123,7 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A20" s="134"/>
+      <c r="A20" s="135"/>
       <c r="B20" s="52" t="s">
         <v>4</v>
       </c>
@@ -54240,7 +54246,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A21" s="134"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="52" t="s">
         <v>5</v>
       </c>
@@ -54363,7 +54369,7 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A22" s="135"/>
+      <c r="A22" s="136"/>
       <c r="B22" s="54" t="s">
         <v>6</v>
       </c>
@@ -54486,7 +54492,7 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A23" s="134" t="s">
+      <c r="A23" s="135" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="69" t="s">
@@ -54611,7 +54617,7 @@
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A24" s="134"/>
+      <c r="A24" s="135"/>
       <c r="B24" s="52" t="s">
         <v>8</v>
       </c>
@@ -54734,7 +54740,7 @@
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A25" s="134"/>
+      <c r="A25" s="135"/>
       <c r="B25" s="52" t="s">
         <v>14</v>
       </c>
@@ -54857,7 +54863,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A26" s="134"/>
+      <c r="A26" s="135"/>
       <c r="B26" s="52" t="s">
         <v>11</v>
       </c>
@@ -54980,7 +54986,7 @@
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A27" s="134"/>
+      <c r="A27" s="135"/>
       <c r="B27" s="52" t="s">
         <v>13</v>
       </c>
@@ -55103,7 +55109,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A28" s="134"/>
+      <c r="A28" s="135"/>
       <c r="B28" s="52" t="s">
         <v>5</v>
       </c>
@@ -55226,7 +55232,7 @@
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A29" s="134"/>
+      <c r="A29" s="135"/>
       <c r="B29" s="52" t="s">
         <v>0</v>
       </c>
@@ -55349,7 +55355,7 @@
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A30" s="134"/>
+      <c r="A30" s="135"/>
       <c r="B30" s="52" t="s">
         <v>1</v>
       </c>
@@ -55472,7 +55478,7 @@
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A31" s="134"/>
+      <c r="A31" s="135"/>
       <c r="B31" s="53" t="s">
         <v>18</v>
       </c>
@@ -55595,7 +55601,7 @@
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A32" s="134"/>
+      <c r="A32" s="135"/>
       <c r="B32" s="52" t="s">
         <v>19</v>
       </c>
@@ -55718,7 +55724,7 @@
       </c>
     </row>
     <row r="33" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A33" s="134"/>
+      <c r="A33" s="135"/>
       <c r="B33" s="52" t="s">
         <v>2</v>
       </c>
@@ -55841,7 +55847,7 @@
       </c>
     </row>
     <row r="34" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A34" s="134"/>
+      <c r="A34" s="135"/>
       <c r="B34" s="52" t="s">
         <v>3</v>
       </c>
@@ -55964,7 +55970,7 @@
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A35" s="134"/>
+      <c r="A35" s="135"/>
       <c r="B35" s="52" t="s">
         <v>4</v>
       </c>
@@ -56087,7 +56093,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A36" s="134"/>
+      <c r="A36" s="135"/>
       <c r="B36" s="52" t="s">
         <v>5</v>
       </c>
@@ -56210,7 +56216,7 @@
       </c>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A37" s="134"/>
+      <c r="A37" s="135"/>
       <c r="B37" s="54" t="s">
         <v>6</v>
       </c>
@@ -56333,7 +56339,7 @@
       </c>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A38" s="133" t="s">
+      <c r="A38" s="134" t="s">
         <v>51</v>
       </c>
       <c r="B38" s="69" t="s">
@@ -56458,7 +56464,7 @@
       </c>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A39" s="134"/>
+      <c r="A39" s="135"/>
       <c r="B39" s="52" t="s">
         <v>8</v>
       </c>
@@ -56581,7 +56587,7 @@
       </c>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A40" s="134"/>
+      <c r="A40" s="135"/>
       <c r="B40" s="52" t="s">
         <v>15</v>
       </c>
@@ -56704,7 +56710,7 @@
       </c>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A41" s="134"/>
+      <c r="A41" s="135"/>
       <c r="B41" s="52" t="s">
         <v>11</v>
       </c>
@@ -56827,7 +56833,7 @@
       </c>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A42" s="134"/>
+      <c r="A42" s="135"/>
       <c r="B42" s="52" t="s">
         <v>16</v>
       </c>
@@ -56950,7 +56956,7 @@
       </c>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A43" s="134"/>
+      <c r="A43" s="135"/>
       <c r="B43" s="52" t="s">
         <v>17</v>
       </c>
@@ -57073,7 +57079,7 @@
       </c>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A44" s="134"/>
+      <c r="A44" s="135"/>
       <c r="B44" s="52" t="s">
         <v>0</v>
       </c>
@@ -57196,7 +57202,7 @@
       </c>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A45" s="134"/>
+      <c r="A45" s="135"/>
       <c r="B45" s="52" t="s">
         <v>1</v>
       </c>
@@ -57319,7 +57325,7 @@
       </c>
     </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A46" s="134"/>
+      <c r="A46" s="135"/>
       <c r="B46" s="53" t="s">
         <v>18</v>
       </c>
@@ -57442,7 +57448,7 @@
       </c>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A47" s="134"/>
+      <c r="A47" s="135"/>
       <c r="B47" s="52" t="s">
         <v>19</v>
       </c>
@@ -57565,7 +57571,7 @@
       </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A48" s="134"/>
+      <c r="A48" s="135"/>
       <c r="B48" s="52" t="s">
         <v>2</v>
       </c>
@@ -57688,7 +57694,7 @@
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A49" s="134"/>
+      <c r="A49" s="135"/>
       <c r="B49" s="52" t="s">
         <v>3</v>
       </c>
@@ -57811,7 +57817,7 @@
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A50" s="134"/>
+      <c r="A50" s="135"/>
       <c r="B50" s="52" t="s">
         <v>4</v>
       </c>
@@ -57934,7 +57940,7 @@
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A51" s="134"/>
+      <c r="A51" s="135"/>
       <c r="B51" s="52" t="s">
         <v>5</v>
       </c>
@@ -58057,7 +58063,7 @@
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A52" s="134"/>
+      <c r="A52" s="135"/>
       <c r="B52" s="52" t="s">
         <v>6</v>
       </c>
@@ -58180,7 +58186,7 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A53" s="135"/>
+      <c r="A53" s="136"/>
       <c r="B53" s="54" t="s">
         <v>7</v>
       </c>
@@ -58329,7 +58335,7 @@
   </sheetPr>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -58347,11 +58353,11 @@
       <c r="A1" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="67"/>
       <c r="F1" s="67"/>
       <c r="G1" s="68"/>
@@ -58359,10 +58365,10 @@
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="127"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="34" t="s">
         <v>57</v>
       </c>
@@ -58374,10 +58380,10 @@
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="128"/>
+      <c r="B3" s="129"/>
       <c r="C3" s="34"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -58398,24 +58404,24 @@
       <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="140" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="141" t="s">
+      <c r="C5" s="141"/>
+      <c r="D5" s="142" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="142"/>
-      <c r="F5" s="143" t="s">
+      <c r="E5" s="143"/>
+      <c r="F5" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="144"/>
+      <c r="G5" s="145"/>
     </row>
     <row r="6" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="138"/>
+      <c r="A6" s="139"/>
       <c r="B6" s="35" t="s">
         <v>103</v>
       </c>
@@ -58641,11 +58647,11 @@
       <c r="G15" s="2">
         <v>1159</v>
       </c>
-      <c r="I15" s="155">
+      <c r="I15" s="122">
         <f>D15-E15</f>
         <v>1580</v>
       </c>
-      <c r="J15" s="155">
+      <c r="J15" s="122">
         <f>F15-G15</f>
         <v>3286</v>
       </c>
@@ -58672,11 +58678,11 @@
       <c r="G16" s="2">
         <v>1154</v>
       </c>
-      <c r="I16" s="155">
+      <c r="I16" s="122">
         <f t="shared" ref="I16:I44" si="0">D16-E16</f>
         <v>1569</v>
       </c>
-      <c r="J16" s="155">
+      <c r="J16" s="122">
         <f t="shared" ref="J16:J44" si="1">F16-G16</f>
         <v>2743</v>
       </c>
@@ -58703,11 +58709,11 @@
       <c r="G17" s="2">
         <v>1138</v>
       </c>
-      <c r="I17" s="155">
+      <c r="I17" s="122">
         <f t="shared" si="0"/>
         <v>1572</v>
       </c>
-      <c r="J17" s="155">
+      <c r="J17" s="122">
         <f t="shared" si="1"/>
         <v>2381</v>
       </c>
@@ -58734,11 +58740,11 @@
       <c r="G18" s="2">
         <v>1143</v>
       </c>
-      <c r="I18" s="155">
+      <c r="I18" s="122">
         <f t="shared" si="0"/>
         <v>1585</v>
       </c>
-      <c r="J18" s="155">
+      <c r="J18" s="122">
         <f t="shared" si="1"/>
         <v>2245</v>
       </c>
@@ -58765,11 +58771,11 @@
       <c r="G19" s="2">
         <v>1131</v>
       </c>
-      <c r="I19" s="155">
+      <c r="I19" s="122">
         <f t="shared" si="0"/>
         <v>1562</v>
       </c>
-      <c r="J19" s="155">
+      <c r="J19" s="122">
         <f t="shared" si="1"/>
         <v>2283</v>
       </c>
@@ -58796,11 +58802,11 @@
       <c r="G20" s="2">
         <v>1128</v>
       </c>
-      <c r="I20" s="155">
+      <c r="I20" s="122">
         <f t="shared" si="0"/>
         <v>1556</v>
       </c>
-      <c r="J20" s="155">
+      <c r="J20" s="122">
         <f t="shared" si="1"/>
         <v>2314</v>
       </c>
@@ -58827,11 +58833,11 @@
       <c r="G21" s="2">
         <v>1109</v>
       </c>
-      <c r="I21" s="155">
+      <c r="I21" s="122">
         <f t="shared" si="0"/>
         <v>1580</v>
       </c>
-      <c r="J21" s="155">
+      <c r="J21" s="122">
         <f t="shared" si="1"/>
         <v>2369</v>
       </c>
@@ -58858,11 +58864,11 @@
       <c r="G22" s="2">
         <v>1093</v>
       </c>
-      <c r="I22" s="155">
+      <c r="I22" s="122">
         <f t="shared" si="0"/>
         <v>1568</v>
       </c>
-      <c r="J22" s="155">
+      <c r="J22" s="122">
         <f t="shared" si="1"/>
         <v>2414</v>
       </c>
@@ -58889,11 +58895,11 @@
       <c r="G23" s="2">
         <v>1084</v>
       </c>
-      <c r="I23" s="155">
+      <c r="I23" s="122">
         <f t="shared" si="0"/>
         <v>1512</v>
       </c>
-      <c r="J23" s="155">
+      <c r="J23" s="122">
         <f t="shared" si="1"/>
         <v>2461</v>
       </c>
@@ -58920,11 +58926,11 @@
       <c r="G24" s="2">
         <v>1071</v>
       </c>
-      <c r="I24" s="155">
+      <c r="I24" s="122">
         <f t="shared" si="0"/>
         <v>1491</v>
       </c>
-      <c r="J24" s="155">
+      <c r="J24" s="122">
         <f t="shared" si="1"/>
         <v>2501</v>
       </c>
@@ -58951,11 +58957,11 @@
       <c r="G25" s="2">
         <v>1074</v>
       </c>
-      <c r="I25" s="155">
+      <c r="I25" s="122">
         <f t="shared" si="0"/>
         <v>1458</v>
       </c>
-      <c r="J25" s="155">
+      <c r="J25" s="122">
         <f t="shared" si="1"/>
         <v>2528</v>
       </c>
@@ -58982,11 +58988,11 @@
       <c r="G26" s="2">
         <v>1075</v>
       </c>
-      <c r="I26" s="155">
+      <c r="I26" s="122">
         <f t="shared" si="0"/>
         <v>1398</v>
       </c>
-      <c r="J26" s="155">
+      <c r="J26" s="122">
         <f t="shared" si="1"/>
         <v>2561</v>
       </c>
@@ -59013,11 +59019,11 @@
       <c r="G27" s="2">
         <v>1067</v>
       </c>
-      <c r="I27" s="155">
+      <c r="I27" s="122">
         <f t="shared" si="0"/>
         <v>1346</v>
       </c>
-      <c r="J27" s="155">
+      <c r="J27" s="122">
         <f t="shared" si="1"/>
         <v>2606</v>
       </c>
@@ -59044,11 +59050,11 @@
       <c r="G28" s="2">
         <v>1056</v>
       </c>
-      <c r="I28" s="155">
+      <c r="I28" s="122">
         <f t="shared" si="0"/>
         <v>1326</v>
       </c>
-      <c r="J28" s="155">
+      <c r="J28" s="122">
         <f t="shared" si="1"/>
         <v>2647</v>
       </c>
@@ -59075,11 +59081,11 @@
       <c r="G29" s="2">
         <v>1053</v>
       </c>
-      <c r="I29" s="155">
+      <c r="I29" s="122">
         <f t="shared" si="0"/>
         <v>1231</v>
       </c>
-      <c r="J29" s="155">
+      <c r="J29" s="122">
         <f t="shared" si="1"/>
         <v>2678</v>
       </c>
@@ -59106,11 +59112,11 @@
       <c r="G30" s="2">
         <v>1044</v>
       </c>
-      <c r="I30" s="155">
+      <c r="I30" s="122">
         <f t="shared" si="0"/>
         <v>1154</v>
       </c>
-      <c r="J30" s="155">
+      <c r="J30" s="122">
         <f t="shared" si="1"/>
         <v>2709</v>
       </c>
@@ -59137,11 +59143,11 @@
       <c r="G31" s="2">
         <v>1042</v>
       </c>
-      <c r="I31" s="155">
+      <c r="I31" s="122">
         <f t="shared" si="0"/>
         <v>1063</v>
       </c>
-      <c r="J31" s="155">
+      <c r="J31" s="122">
         <f t="shared" si="1"/>
         <v>2736</v>
       </c>
@@ -59168,11 +59174,11 @@
       <c r="G32" s="2">
         <v>1037</v>
       </c>
-      <c r="I32" s="155">
+      <c r="I32" s="122">
         <f t="shared" si="0"/>
         <v>922</v>
       </c>
-      <c r="J32" s="155">
+      <c r="J32" s="122">
         <f t="shared" si="1"/>
         <v>2767</v>
       </c>
@@ -59199,11 +59205,11 @@
       <c r="G33" s="2">
         <v>1029</v>
       </c>
-      <c r="I33" s="155">
+      <c r="I33" s="122">
         <f t="shared" si="0"/>
         <v>806</v>
       </c>
-      <c r="J33" s="155">
+      <c r="J33" s="122">
         <f t="shared" si="1"/>
         <v>2788</v>
       </c>
@@ -59230,11 +59236,11 @@
       <c r="G34" s="2">
         <v>1030</v>
       </c>
-      <c r="I34" s="155">
+      <c r="I34" s="122">
         <f t="shared" si="0"/>
         <v>693</v>
       </c>
-      <c r="J34" s="155">
+      <c r="J34" s="122">
         <f t="shared" si="1"/>
         <v>2802</v>
       </c>
@@ -59261,11 +59267,11 @@
       <c r="G35" s="2">
         <v>1026</v>
       </c>
-      <c r="I35" s="155">
+      <c r="I35" s="122">
         <f t="shared" si="0"/>
         <v>566</v>
       </c>
-      <c r="J35" s="155">
+      <c r="J35" s="122">
         <f t="shared" si="1"/>
         <v>2824</v>
       </c>
@@ -59292,11 +59298,11 @@
       <c r="G36" s="2">
         <v>1017</v>
       </c>
-      <c r="I36" s="155">
+      <c r="I36" s="122">
         <f t="shared" si="0"/>
         <v>449</v>
       </c>
-      <c r="J36" s="155">
+      <c r="J36" s="122">
         <f t="shared" si="1"/>
         <v>2856</v>
       </c>
@@ -59323,11 +59329,11 @@
       <c r="G37" s="2">
         <v>1015</v>
       </c>
-      <c r="I37" s="155">
+      <c r="I37" s="122">
         <f t="shared" si="0"/>
         <v>315</v>
       </c>
-      <c r="J37" s="155">
+      <c r="J37" s="122">
         <f t="shared" si="1"/>
         <v>2873</v>
       </c>
@@ -59354,11 +59360,11 @@
       <c r="G38" s="2">
         <v>1005</v>
       </c>
-      <c r="I38" s="155">
+      <c r="I38" s="122">
         <f t="shared" si="0"/>
         <v>223</v>
       </c>
-      <c r="J38" s="155">
+      <c r="J38" s="122">
         <f t="shared" si="1"/>
         <v>2894</v>
       </c>
@@ -59385,11 +59391,11 @@
       <c r="G39" s="2">
         <v>1007</v>
       </c>
-      <c r="I39" s="155">
+      <c r="I39" s="122">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="J39" s="155">
+      <c r="J39" s="122">
         <f t="shared" si="1"/>
         <v>2913</v>
       </c>
@@ -59416,11 +59422,11 @@
       <c r="G40" s="2">
         <v>1005</v>
       </c>
-      <c r="I40" s="155">
+      <c r="I40" s="122">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="J40" s="155">
+      <c r="J40" s="122">
         <f t="shared" si="1"/>
         <v>2936</v>
       </c>
@@ -59447,11 +59453,11 @@
       <c r="G41" s="2">
         <v>1001</v>
       </c>
-      <c r="I41" s="155">
+      <c r="I41" s="122">
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-      <c r="J41" s="155">
+      <c r="J41" s="122">
         <f t="shared" si="1"/>
         <v>2951</v>
       </c>
@@ -59478,11 +59484,11 @@
       <c r="G42" s="2">
         <v>995</v>
       </c>
-      <c r="I42" s="155">
+      <c r="I42" s="122">
         <f t="shared" si="0"/>
         <v>-70</v>
       </c>
-      <c r="J42" s="155">
+      <c r="J42" s="122">
         <f t="shared" si="1"/>
         <v>2968</v>
       </c>
@@ -59509,11 +59515,11 @@
       <c r="G43" s="2">
         <v>990</v>
       </c>
-      <c r="I43" s="155">
+      <c r="I43" s="122">
         <f>D43-E43</f>
         <v>-99</v>
       </c>
-      <c r="J43" s="155">
+      <c r="J43" s="122">
         <f t="shared" si="1"/>
         <v>2984</v>
       </c>
@@ -59540,11 +59546,11 @@
       <c r="G44" s="6">
         <v>994</v>
       </c>
-      <c r="I44" s="155">
+      <c r="I44" s="122">
         <f t="shared" si="0"/>
         <v>-152</v>
       </c>
-      <c r="J44" s="155">
+      <c r="J44" s="122">
         <f t="shared" si="1"/>
         <v>2992</v>
       </c>
@@ -59595,10 +59601,10 @@
   <sheetData>
     <row r="1" spans="1:39" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="117"/>
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="147" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="147"/>
+      <c r="C1" s="148"/>
       <c r="D1" s="102"/>
       <c r="E1" s="102"/>
       <c r="F1" s="102"/>
@@ -59640,10 +59646,10 @@
       <c r="A2" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="149" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="149"/>
+      <c r="C2" s="150"/>
       <c r="D2" s="101"/>
       <c r="E2" s="101"/>
       <c r="F2" s="101"/>
@@ -59685,8 +59691,8 @@
       <c r="A3" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="150"/>
-      <c r="C3" s="151"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="101"/>
       <c r="E3" s="101"/>
       <c r="F3" s="101"/>
@@ -59723,11 +59729,11 @@
       <c r="AM3" s="105"/>
     </row>
     <row r="4" spans="1:39" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="153"/>
-      <c r="C4" s="154"/>
+      <c r="B4" s="154"/>
+      <c r="C4" s="155"/>
       <c r="I4" s="91"/>
       <c r="J4" s="91"/>
       <c r="P4" s="87"/>

</xml_diff>